<commit_message>
changed diad1 and diad2 fitting to be much more similar
</commit_message>
<xml_diff>
--- a/docs/Examples/Diad_Fitting_Nov22nd2022/Med_Diads.xlsx
+++ b/docs/Examples/Diad_Fitting_Nov22nd2022/Med_Diads.xlsx
@@ -537,58 +537,58 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>104.4420457216254</v>
+        <v>104.4425746990862</v>
       </c>
       <c r="D2">
-        <v>1282.730855448159</v>
+        <v>1282.730868820775</v>
       </c>
       <c r="E2">
-        <v>14906.61073714457</v>
+        <v>14906.39371105165</v>
       </c>
       <c r="F2">
-        <v>1282.730705440658</v>
+        <v>1282.730718813274</v>
       </c>
       <c r="G2">
-        <v>44955.71698445117</v>
+        <v>44947.63800973798</v>
       </c>
       <c r="H2">
-        <v>1.10702937399405</v>
+        <v>1.10702453768404</v>
       </c>
       <c r="J2">
-        <v>18.51464699293281</v>
+        <v>18.49878234783836</v>
       </c>
       <c r="K2">
-        <v>0.6930654981862772</v>
+        <v>0.6927723515641337</v>
       </c>
       <c r="L2" t="b">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1387.172801164784</v>
+        <v>1387.17314350486</v>
       </c>
       <c r="N2">
-        <v>29357.98397284797</v>
+        <v>29421.8001272939</v>
       </c>
       <c r="O2">
-        <v>1387.172751162284</v>
+        <v>1387.17329351236</v>
       </c>
       <c r="P2">
-        <v>79281.14264605628</v>
+        <v>80804.4521471122</v>
       </c>
       <c r="Q2">
-        <v>0.9799983846644957</v>
+        <v>0.9781771705224789</v>
       </c>
       <c r="S2">
-        <v>21.38430985117153</v>
+        <v>41.97131683209776</v>
       </c>
       <c r="T2">
-        <v>0.7175065749918462</v>
+        <v>0.7554541260111384</v>
       </c>
       <c r="U2" t="b">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>1262.675794474062</v>
+        <v>1262.674645098945</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -599,58 +599,58 @@
         <v>22</v>
       </c>
       <c r="C3">
-        <v>104.9517543270895</v>
+        <v>104.9481986106382</v>
       </c>
       <c r="D3">
-        <v>1281.779486494736</v>
+        <v>1281.782461697167</v>
       </c>
       <c r="E3">
-        <v>21389.2457076311</v>
+        <v>19888.94515174412</v>
       </c>
       <c r="F3">
-        <v>1281.778136427233</v>
+        <v>1281.782411694667</v>
       </c>
       <c r="G3">
-        <v>31700.81571440438</v>
+        <v>59001.91880459722</v>
       </c>
       <c r="H3">
-        <v>0.6548977137346017</v>
+        <v>1.071728699732787</v>
       </c>
       <c r="J3">
-        <v>174.2640365799156</v>
+        <v>27.54146420985196</v>
       </c>
       <c r="K3">
-        <v>0.9999999999605098</v>
+        <v>0.7429136612205511</v>
       </c>
       <c r="L3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1386.730140766823</v>
+        <v>1386.730660307805</v>
       </c>
       <c r="N3">
-        <v>38205.88127064858</v>
+        <v>38315.77779261894</v>
       </c>
       <c r="O3">
-        <v>1386.729890754322</v>
+        <v>1386.730610305305</v>
       </c>
       <c r="P3">
-        <v>107496.2609118489</v>
+        <v>110782.833857773</v>
       </c>
       <c r="Q3">
-        <v>1.032675369722284</v>
+        <v>1.031879739104645</v>
       </c>
       <c r="S3">
-        <v>135.0814526537793</v>
+        <v>29.36096108578936</v>
       </c>
       <c r="T3">
-        <v>0.7105427667760436</v>
+        <v>0.7630173464862076</v>
       </c>
       <c r="U3" t="b">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>1261.679398243047</v>
+        <v>1261.760056663317</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -661,58 +661,58 @@
         <v>23</v>
       </c>
       <c r="C4">
-        <v>104.5293672730711</v>
+        <v>104.5378114030855</v>
       </c>
       <c r="D4">
-        <v>1282.556570194255</v>
+        <v>1282.549917620856</v>
       </c>
       <c r="E4">
-        <v>26070.73928872314</v>
+        <v>26125.69411200816</v>
       </c>
       <c r="F4">
-        <v>1282.556420186755</v>
+        <v>1282.547067478349</v>
       </c>
       <c r="G4">
-        <v>77581.91930443801</v>
+        <v>77936.44893853911</v>
       </c>
       <c r="H4">
-        <v>1.096547770560167</v>
+        <v>1.0898720731134</v>
       </c>
       <c r="J4">
-        <v>36.40241913893679</v>
+        <v>47.50709129768414</v>
       </c>
       <c r="K4">
-        <v>0.6874427009391118</v>
+        <v>0.7108862664864701</v>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1387.085537447325</v>
+        <v>1387.084928883934</v>
       </c>
       <c r="N4">
-        <v>50656.5838518718</v>
+        <v>50877.91180974832</v>
       </c>
       <c r="O4">
-        <v>1387.085787459826</v>
+        <v>1387.084878881434</v>
       </c>
       <c r="P4">
-        <v>104320.6439885881</v>
+        <v>138781.5532367061</v>
       </c>
       <c r="Q4">
-        <v>0.9263936002379052</v>
+        <v>0.9919617373911227</v>
       </c>
       <c r="S4">
-        <v>109.435536362217</v>
+        <v>38.83076522581072</v>
       </c>
       <c r="T4">
-        <v>0.4482507598684272</v>
+        <v>0.7139670186414619</v>
       </c>
       <c r="U4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1262.501070872692</v>
+        <v>1262.594382681717</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -723,58 +723,58 @@
         <v>24</v>
       </c>
       <c r="C5">
-        <v>104.5929690812816</v>
+        <v>104.5928468061729</v>
       </c>
       <c r="D5">
-        <v>1282.422382586497</v>
+        <v>1282.422381017461</v>
       </c>
       <c r="E5">
-        <v>27783.19692208568</v>
+        <v>27783.20867138372</v>
       </c>
       <c r="F5">
-        <v>1282.422232578997</v>
+        <v>1282.422231009961</v>
       </c>
       <c r="G5">
-        <v>82188.5806841131</v>
+        <v>82189.03412892266</v>
       </c>
       <c r="H5">
-        <v>1.086462279129131</v>
+        <v>1.086462528188054</v>
       </c>
       <c r="J5">
-        <v>33.2306205463918</v>
+        <v>33.2358927304521</v>
       </c>
       <c r="K5">
-        <v>0.6975575689226341</v>
+        <v>0.6975662738323346</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1387.015251662779</v>
+        <v>1387.015127818634</v>
       </c>
       <c r="N5">
-        <v>53954.18929412546</v>
+        <v>53834.87909182344</v>
       </c>
       <c r="O5">
-        <v>1387.015201660279</v>
+        <v>1387.015077816133</v>
       </c>
       <c r="P5">
-        <v>148564.8944559266</v>
+        <v>145258.6941514138</v>
       </c>
       <c r="Q5">
-        <v>0.9979340525838851</v>
+        <v>0.9989210625014198</v>
       </c>
       <c r="S5">
-        <v>42.63325504099723</v>
+        <v>116.6068168691055</v>
       </c>
       <c r="T5">
-        <v>0.7229734459556858</v>
+        <v>0.6816395068060388</v>
       </c>
       <c r="U5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>1262.422277275891</v>
+        <v>1262.422318144928</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -785,58 +785,58 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>104.6482627370051</v>
+        <v>104.6487359290154</v>
       </c>
       <c r="D6">
-        <v>1282.315661486527</v>
+        <v>1282.315324617347</v>
       </c>
       <c r="E6">
-        <v>28634.79983067787</v>
+        <v>28729.21125653609</v>
       </c>
       <c r="F6">
-        <v>1282.315811494027</v>
+        <v>1282.315374619847</v>
       </c>
       <c r="G6">
-        <v>84498.37117675782</v>
+        <v>87787.2242002834</v>
       </c>
       <c r="H6">
-        <v>1.08293129456009</v>
+        <v>1.082845221236768</v>
       </c>
       <c r="J6">
-        <v>42.47576118174936</v>
+        <v>57.28451394872647</v>
       </c>
       <c r="K6">
-        <v>0.7002197559497308</v>
+        <v>0.7652797283714029</v>
       </c>
       <c r="L6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1386.964124233532</v>
+        <v>1386.964160551363</v>
       </c>
       <c r="N6">
-        <v>55425.73641720773</v>
+        <v>55424.39769154091</v>
       </c>
       <c r="O6">
-        <v>1386.964074231032</v>
+        <v>1386.964110548863</v>
       </c>
       <c r="P6">
-        <v>153600.2660394458</v>
+        <v>153558.3155044282</v>
       </c>
       <c r="Q6">
-        <v>1.003896917743509</v>
+        <v>1.003900504424702</v>
       </c>
       <c r="S6">
-        <v>43.11836733240913</v>
+        <v>45.39056612562766</v>
       </c>
       <c r="T6">
-        <v>0.7247502951306868</v>
+        <v>0.7242722724176467</v>
       </c>
       <c r="U6" t="b">
         <v>0</v>
       </c>
       <c r="V6">
-        <v>1262.191823061559</v>
+        <v>1262.358228537804</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -847,58 +847,58 @@
         <v>26</v>
       </c>
       <c r="C7">
-        <v>104.7013214728456</v>
+        <v>104.7006076909645</v>
       </c>
       <c r="D7">
-        <v>1282.221382575133</v>
+        <v>1282.221380320299</v>
       </c>
       <c r="E7">
-        <v>28849.94083212369</v>
+        <v>28849.95166788357</v>
       </c>
       <c r="F7">
-        <v>1282.221332572633</v>
+        <v>1282.221330317799</v>
       </c>
       <c r="G7">
-        <v>84972.64285972182</v>
+        <v>84972.86807868385</v>
       </c>
       <c r="H7">
-        <v>1.075852574201991</v>
+        <v>1.075852099807332</v>
       </c>
       <c r="J7">
-        <v>35.12648086740483</v>
+        <v>35.13569201322791</v>
       </c>
       <c r="K7">
-        <v>0.7121168838918615</v>
+        <v>0.712122562219541</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1386.922504037978</v>
+        <v>1386.921988011264</v>
       </c>
       <c r="N7">
-        <v>55519.81321001017</v>
+        <v>55482.68370309147</v>
       </c>
       <c r="O7">
-        <v>1386.922654045479</v>
+        <v>1386.921938008764</v>
       </c>
       <c r="P7">
-        <v>156135.130130299</v>
+        <v>154793.7462892019</v>
       </c>
       <c r="Q7">
-        <v>1.01092902241861</v>
+        <v>1.010704127227788</v>
       </c>
       <c r="S7">
-        <v>83.62330366562358</v>
+        <v>49.55675165777669</v>
       </c>
       <c r="T7">
-        <v>0.7403623714093247</v>
+        <v>0.7263464159974007</v>
       </c>
       <c r="U7" t="b">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>1262.17215700099</v>
+        <v>1262.172490665632</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -909,58 +909,58 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <v>104.8864630705255</v>
+        <v>104.8871729540144</v>
       </c>
       <c r="D8">
-        <v>1281.88868342265</v>
+        <v>1281.888682685162</v>
       </c>
       <c r="E8">
-        <v>30295.70013415089</v>
+        <v>30295.70183096123</v>
       </c>
       <c r="F8">
-        <v>1281.888533415149</v>
+        <v>1281.888532677662</v>
       </c>
       <c r="G8">
-        <v>89463.11393408255</v>
+        <v>89463.15198056828</v>
       </c>
       <c r="H8">
-        <v>1.071076471736551</v>
+        <v>1.071076413346379</v>
       </c>
       <c r="J8">
-        <v>39.42027922472725</v>
+        <v>39.42431652554543</v>
       </c>
       <c r="K8">
-        <v>0.7332660656887664</v>
+        <v>0.7332669497009476</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1386.775146493175</v>
+        <v>1386.775755634176</v>
       </c>
       <c r="N8">
-        <v>58101.93491823035</v>
+        <v>58207.23499135145</v>
       </c>
       <c r="O8">
-        <v>1386.774996485675</v>
+        <v>1386.775705631676</v>
       </c>
       <c r="P8">
-        <v>163540.6954999112</v>
+        <v>166953.0284489367</v>
       </c>
       <c r="Q8">
-        <v>1.026364694481617</v>
+        <v>1.026371972833134</v>
       </c>
       <c r="S8">
-        <v>188.3077414504907</v>
+        <v>45.81480602016917</v>
       </c>
       <c r="T8">
-        <v>0.7214364878674259</v>
+        <v>0.7560447810855629</v>
       </c>
       <c r="U8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>1261.867086159936</v>
+        <v>1261.86722328511</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -971,58 +971,58 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>104.8002535039266</v>
+        <v>104.80945106739</v>
       </c>
       <c r="D9">
-        <v>1282.037620972327</v>
+        <v>1282.031124675205</v>
       </c>
       <c r="E9">
-        <v>29803.69002668603</v>
+        <v>29858.49283846282</v>
       </c>
       <c r="F9">
-        <v>1282.037770979827</v>
+        <v>1282.0291745777</v>
       </c>
       <c r="G9">
-        <v>88244.00371738766</v>
+        <v>89472.55024240245</v>
       </c>
       <c r="H9">
-        <v>1.074014636139708</v>
+        <v>1.071501073374309</v>
       </c>
       <c r="J9">
-        <v>43.61847816278893</v>
+        <v>57.15751791713139</v>
       </c>
       <c r="K9">
-        <v>0.7280665201600479</v>
+        <v>0.753990971408187</v>
       </c>
       <c r="L9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1386.838174491254</v>
+        <v>1386.83867564759</v>
       </c>
       <c r="N9">
-        <v>57070.57318615889</v>
+        <v>57197.89006521182</v>
       </c>
       <c r="O9">
-        <v>1386.838024483754</v>
+        <v>1386.83862564509</v>
       </c>
       <c r="P9">
-        <v>158264.9553419318</v>
+        <v>162241.5092842063</v>
       </c>
       <c r="Q9">
-        <v>1.021603174711842</v>
+        <v>1.021358859110689</v>
       </c>
       <c r="S9">
-        <v>193.228619270613</v>
+        <v>46.31357694180411</v>
       </c>
       <c r="T9">
-        <v>0.6978407464197534</v>
+        <v>0.7405643240705246</v>
       </c>
       <c r="U9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>1261.920404082935</v>
+        <v>1262.174421049026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaks most inputs based on Scipy find peaks.
</commit_message>
<xml_diff>
--- a/docs/Examples/Diad_Fitting_Nov22nd2022/Med_Diads.xlsx
+++ b/docs/Examples/Diad_Fitting_Nov22nd2022/Med_Diads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
   <si>
     <t>filename</t>
   </si>
@@ -106,97 +106,82 @@
     <t>C13_Sigma</t>
   </si>
   <si>
-    <t>POC39</t>
+    <t>POC10</t>
+  </si>
+  <si>
+    <t>POC11</t>
+  </si>
+  <si>
+    <t>POC12</t>
+  </si>
+  <si>
+    <t>POC13</t>
+  </si>
+  <si>
+    <t>POC14</t>
+  </si>
+  <si>
+    <t>POC15</t>
+  </si>
+  <si>
+    <t>POC16</t>
+  </si>
+  <si>
+    <t>POC17</t>
+  </si>
+  <si>
+    <t>POC18</t>
+  </si>
+  <si>
+    <t>POC19</t>
+  </si>
+  <si>
+    <t>POC20</t>
+  </si>
+  <si>
+    <t>POC21</t>
+  </si>
+  <si>
+    <t>POC22</t>
+  </si>
+  <si>
+    <t>POC23</t>
+  </si>
+  <si>
+    <t>POC24</t>
+  </si>
+  <si>
+    <t>POC25</t>
+  </si>
+  <si>
+    <t>POC26</t>
+  </si>
+  <si>
+    <t>POC27</t>
+  </si>
+  <si>
+    <t>POC28</t>
+  </si>
+  <si>
+    <t>POC29</t>
   </si>
   <si>
     <t>POC30</t>
   </si>
   <si>
-    <t>POC38</t>
-  </si>
-  <si>
-    <t>POC20</t>
-  </si>
-  <si>
-    <t>POC29</t>
-  </si>
-  <si>
-    <t>POC37</t>
-  </si>
-  <si>
-    <t>POC19</t>
-  </si>
-  <si>
-    <t>POC25</t>
-  </si>
-  <si>
-    <t>POC26</t>
-  </si>
-  <si>
-    <t>POC24</t>
-  </si>
-  <si>
-    <t>POC23</t>
-  </si>
-  <si>
-    <t>POC28</t>
-  </si>
-  <si>
-    <t>POC18</t>
-  </si>
-  <si>
-    <t>POC22</t>
-  </si>
-  <si>
-    <t>POC27</t>
-  </si>
-  <si>
-    <t>POC21</t>
-  </si>
-  <si>
-    <t>POC36</t>
-  </si>
-  <si>
-    <t>POC17</t>
-  </si>
-  <si>
-    <t>POC35</t>
-  </si>
-  <si>
-    <t>POC11</t>
-  </si>
-  <si>
-    <t>POC16</t>
-  </si>
-  <si>
-    <t>POC15</t>
+    <t>POC31</t>
+  </si>
+  <si>
+    <t>POC32</t>
+  </si>
+  <si>
+    <t>POC33</t>
   </si>
   <si>
     <t>POC34</t>
   </si>
   <si>
-    <t>POC10</t>
-  </si>
-  <si>
     <t>POC9</t>
-  </si>
-  <si>
-    <t>POC14</t>
-  </si>
-  <si>
-    <t>POC13</t>
-  </si>
-  <si>
-    <t>POC33</t>
-  </si>
-  <si>
-    <t>POC12</t>
-  </si>
-  <si>
-    <t>POC32</t>
-  </si>
-  <si>
-    <t>POC31</t>
   </si>
   <si>
     <t>Flagged Warnings:</t>
@@ -557,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,79 +648,88 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>102.8074953906628</v>
+        <v>104.3059996367085</v>
       </c>
       <c r="D2">
-        <v>1286.514192219764</v>
+        <v>1283.014021678285</v>
       </c>
       <c r="E2">
-        <v>2008.16155270561</v>
+        <v>3849.242921342655</v>
       </c>
       <c r="F2">
-        <v>1286.514242222265</v>
+        <v>1283.014071680785</v>
       </c>
       <c r="G2">
-        <v>3118.221074646824</v>
+        <v>12062.05972617332</v>
       </c>
       <c r="H2">
-        <v>0.6527423720692442</v>
+        <v>1.133925370955545</v>
       </c>
       <c r="I2">
-        <v>4.974766250798933</v>
+        <v>7.6219791614992</v>
       </c>
       <c r="J2">
-        <v>0.326100702985937</v>
+        <v>0.7149602092136067</v>
       </c>
       <c r="K2">
-        <v>1.305484744138488</v>
+        <v>2.267850741911091</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M2">
-        <v>1389.321787615427</v>
+        <v>1387.320121319994</v>
       </c>
       <c r="N2">
-        <v>3154.228138754199</v>
+        <v>7636.769307514072</v>
       </c>
       <c r="O2">
-        <v>1389.321737612927</v>
+        <v>1387.320071317494</v>
       </c>
       <c r="P2">
-        <v>4505.207530283971</v>
+        <v>20280.39786734401</v>
       </c>
       <c r="Q2">
-        <v>0.6018936416649683</v>
+        <v>0.9749778703838463</v>
       </c>
       <c r="S2">
-        <v>5.512164808480862</v>
+        <v>6.462544976457504</v>
       </c>
       <c r="T2">
-        <v>0.3191827545186863</v>
+        <v>0.6885793416078102</v>
       </c>
       <c r="U2">
-        <v>1.203787283329937</v>
+        <v>1.949955740767693</v>
       </c>
       <c r="V2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W2">
-        <v>1266.22770112946</v>
+        <v>1262.979849043113</v>
       </c>
       <c r="X2">
-        <v>327.6573971884865</v>
+        <v>1763.210061234113</v>
       </c>
       <c r="Y2">
-        <v>0.7477442792188347</v>
+        <v>3.040690309620107</v>
       </c>
       <c r="Z2">
-        <v>1410.567353949535</v>
+        <v>1408.692279507823</v>
       </c>
       <c r="AA2">
-        <v>451.4517571943791</v>
+        <v>2053.602881532134</v>
       </c>
       <c r="AB2">
-        <v>0.6490675155838831</v>
+        <v>2.105387231639656</v>
+      </c>
+      <c r="AC2">
+        <v>1369.669780896665</v>
+      </c>
+      <c r="AD2">
+        <v>262.5348767247454</v>
+      </c>
+      <c r="AE2">
+        <v>0.4861250673680944</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -746,79 +740,88 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>103.1251870487158</v>
+        <v>104.2506869694121</v>
       </c>
       <c r="D3">
-        <v>1285.703696786481</v>
+        <v>1283.138721676644</v>
       </c>
       <c r="E3">
-        <v>2054.555922075671</v>
+        <v>3186.193417624571</v>
       </c>
       <c r="F3">
-        <v>1285.703746788981</v>
+        <v>1283.138771679144</v>
       </c>
       <c r="G3">
-        <v>4358.212268783303</v>
+        <v>10088.13946911944</v>
       </c>
       <c r="H3">
-        <v>0.8212460204481888</v>
+        <v>1.167244489581091</v>
       </c>
       <c r="I3">
-        <v>3.826404944844122</v>
+        <v>6.21685150811758</v>
       </c>
       <c r="J3">
-        <v>0.5458537868349655</v>
+        <v>0.669860284815971</v>
       </c>
       <c r="K3">
-        <v>1.642492040896378</v>
+        <v>2.334488979162181</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M3">
-        <v>1388.828983840197</v>
+        <v>1387.389408646056</v>
       </c>
       <c r="N3">
-        <v>3711.054357034817</v>
+        <v>6469.820418821713</v>
       </c>
       <c r="O3">
-        <v>1388.828933837697</v>
+        <v>1387.389458648556</v>
       </c>
       <c r="P3">
-        <v>6763.282508902012</v>
+        <v>17127.45717351187</v>
       </c>
       <c r="Q3">
-        <v>0.7105480175808048</v>
+        <v>0.9640872897845647</v>
       </c>
       <c r="S3">
-        <v>5.127176387829925</v>
+        <v>5.292381932947681</v>
       </c>
       <c r="T3">
-        <v>0.5275339849058686</v>
+        <v>0.7066149169089692</v>
       </c>
       <c r="U3">
-        <v>1.42109603516161</v>
+        <v>1.928174579569129</v>
       </c>
       <c r="V3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W3">
-        <v>1265.550055586745</v>
+        <v>1263.120274632635</v>
       </c>
       <c r="X3">
-        <v>494.7951848154528</v>
+        <v>1408.037424774914</v>
       </c>
       <c r="Y3">
-        <v>1.120399396588809</v>
+        <v>2.849476266432021</v>
       </c>
       <c r="Z3">
-        <v>1410.087447003707</v>
+        <v>1408.758153684715</v>
       </c>
       <c r="AA3">
-        <v>682.2343171916374</v>
+        <v>1846.273564084462</v>
       </c>
       <c r="AB3">
-        <v>0.869486993488</v>
+        <v>2.071863447623134</v>
+      </c>
+      <c r="AC3">
+        <v>1369.725661693554</v>
+      </c>
+      <c r="AD3">
+        <v>211.9950110289869</v>
+      </c>
+      <c r="AE3">
+        <v>0.4808279332425745</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -829,79 +832,88 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>102.811068795065</v>
+        <v>104.1637430559647</v>
       </c>
       <c r="D4">
-        <v>1286.490983827585</v>
+        <v>1283.321140367118</v>
       </c>
       <c r="E4">
-        <v>2228.973771020726</v>
+        <v>4289.980252150035</v>
       </c>
       <c r="F4">
-        <v>1286.491033830085</v>
+        <v>1283.321190369619</v>
       </c>
       <c r="G4">
-        <v>3465.208480212499</v>
+        <v>13687.2667198066</v>
       </c>
       <c r="H4">
-        <v>0.652195149390729</v>
+        <v>1.18755071513728</v>
       </c>
       <c r="I4">
-        <v>4.784158159525784</v>
+        <v>8.4003170191792</v>
       </c>
       <c r="J4">
-        <v>0.331737218430578</v>
+        <v>0.6465344567480427</v>
       </c>
       <c r="K4">
-        <v>1.304390298781458</v>
+        <v>2.37510143027456</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M4">
-        <v>1389.30215262765</v>
+        <v>1387.484883423083</v>
       </c>
       <c r="N4">
-        <v>3450.300432256481</v>
+        <v>8737.113094037666</v>
       </c>
       <c r="O4">
-        <v>1389.30210262515</v>
+        <v>1387.484933425583</v>
       </c>
       <c r="P4">
-        <v>4977.71369500543</v>
+        <v>22925.73656551052</v>
       </c>
       <c r="Q4">
-        <v>0.6106422124908271</v>
+        <v>0.9678034784732368</v>
       </c>
       <c r="S4">
-        <v>5.991580355056961</v>
+        <v>7.362277882051407</v>
       </c>
       <c r="T4">
-        <v>0.3068827953064002</v>
+        <v>0.6762115483937787</v>
       </c>
       <c r="U4">
-        <v>1.221284424981654</v>
+        <v>1.935606956946474</v>
       </c>
       <c r="V4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W4">
-        <v>1266.23292721904</v>
+        <v>1263.259971943284</v>
       </c>
       <c r="X4">
-        <v>362.8654390509474</v>
+        <v>1960.121594704945</v>
       </c>
       <c r="Y4">
-        <v>0.768651790212702</v>
+        <v>2.92017297883555</v>
       </c>
       <c r="Z4">
-        <v>1410.568639440903</v>
+        <v>1408.863249324054</v>
       </c>
       <c r="AA4">
-        <v>501.2395722657766</v>
+        <v>2414.324325120559</v>
       </c>
       <c r="AB4">
-        <v>0.617444954723962</v>
+        <v>1.966275055177676</v>
+      </c>
+      <c r="AC4">
+        <v>1369.725478989538</v>
+      </c>
+      <c r="AD4">
+        <v>289.8432913024593</v>
+      </c>
+      <c r="AE4">
+        <v>0.4826831137636053</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -912,79 +924,88 @@
         <v>33</v>
       </c>
       <c r="C5">
-        <v>103.6685915936514</v>
+        <v>104.1341188474307</v>
       </c>
       <c r="D5">
-        <v>1284.419217325557</v>
+        <v>1283.384531539467</v>
       </c>
       <c r="E5">
-        <v>1861.949083165387</v>
+        <v>4018.856780517452</v>
       </c>
       <c r="F5">
-        <v>1284.419267328057</v>
+        <v>1283.384581541967</v>
       </c>
       <c r="G5">
-        <v>5769.947306055225</v>
+        <v>12935.72215457865</v>
       </c>
       <c r="H5">
-        <v>1.206615026138527</v>
+        <v>1.196464311349655</v>
       </c>
       <c r="I5">
-        <v>4.218625572573188</v>
+        <v>6.963142933002961</v>
       </c>
       <c r="J5">
-        <v>0.5320338463890102</v>
+        <v>0.6496944277286643</v>
       </c>
       <c r="K5">
-        <v>2.413230052277053</v>
+        <v>2.39292862269931</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M5">
-        <v>1388.087908924208</v>
+        <v>1387.518650386898</v>
       </c>
       <c r="N5">
-        <v>3831.187779793816</v>
+        <v>8263.009505846145</v>
       </c>
       <c r="O5">
-        <v>1388.087858921708</v>
+        <v>1387.518700389398</v>
       </c>
       <c r="P5">
-        <v>9456.914181133272</v>
+        <v>21695.96450911216</v>
       </c>
       <c r="Q5">
-        <v>0.9265462520502596</v>
+        <v>0.9701167047332506</v>
       </c>
       <c r="S5">
-        <v>8.99863660669317</v>
+        <v>7.103023733860548</v>
       </c>
       <c r="T5">
-        <v>0.6238959761296917</v>
+        <v>0.6718563926602505</v>
       </c>
       <c r="U5">
-        <v>1.853092504100519</v>
+        <v>1.940233409466501</v>
       </c>
       <c r="V5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W5">
-        <v>1264.362497136706</v>
+        <v>1263.40522527045</v>
       </c>
       <c r="X5">
-        <v>693.4186235997388</v>
+        <v>1833.361872832842</v>
       </c>
       <c r="Y5">
-        <v>1.827023153410534</v>
+        <v>2.766703401929435</v>
       </c>
       <c r="Z5">
-        <v>1409.461577842379</v>
+        <v>1408.878752277463</v>
       </c>
       <c r="AA5">
-        <v>1035.693437021676</v>
+        <v>2291.700382701857</v>
       </c>
       <c r="AB5">
-        <v>1.526142616715261</v>
+        <v>1.955771573840638</v>
+      </c>
+      <c r="AC5">
+        <v>1369.751568077714</v>
+      </c>
+      <c r="AD5">
+        <v>279.6055189399362</v>
+      </c>
+      <c r="AE5">
+        <v>0.4838017148620677</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -995,79 +1016,88 @@
         <v>34</v>
       </c>
       <c r="C6">
-        <v>103.1903200097574</v>
+        <v>104.1084396958004</v>
       </c>
       <c r="D6">
-        <v>1285.554107190773</v>
+        <v>1283.44269231725</v>
       </c>
       <c r="E6">
-        <v>2253.972026466532</v>
+        <v>3728.121021814217</v>
       </c>
       <c r="F6">
-        <v>1285.554157193273</v>
+        <v>1283.44274231975</v>
       </c>
       <c r="G6">
-        <v>4974.551249884729</v>
+        <v>12134.33685055332</v>
       </c>
       <c r="H6">
-        <v>0.8452589278090297</v>
+        <v>1.210279800797113</v>
       </c>
       <c r="I6">
-        <v>3.508382899382292</v>
+        <v>6.465663578071212</v>
       </c>
       <c r="J6">
-        <v>0.5734002210661765</v>
+        <v>0.6488357743405737</v>
       </c>
       <c r="K6">
-        <v>1.690517855618059</v>
+        <v>2.420559601594226</v>
       </c>
       <c r="L6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M6">
-        <v>1388.744527205531</v>
+        <v>1387.551132013051</v>
       </c>
       <c r="N6">
-        <v>4071.371134333878</v>
+        <v>7698.642825072863</v>
       </c>
       <c r="O6">
-        <v>1388.744477203031</v>
+        <v>1387.551182015551</v>
       </c>
       <c r="P6">
-        <v>7707.1451880819</v>
+        <v>20137.73569775269</v>
       </c>
       <c r="Q6">
-        <v>0.7347575534710218</v>
+        <v>0.9669067183327722</v>
       </c>
       <c r="S6">
-        <v>5.757955798616551</v>
+        <v>6.856344412475273</v>
       </c>
       <c r="T6">
-        <v>0.5390728122774033</v>
+        <v>0.6705136115034953</v>
       </c>
       <c r="U6">
-        <v>1.469515106942044</v>
+        <v>1.933813436665544</v>
       </c>
       <c r="V6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W6">
-        <v>1265.42088509884</v>
+        <v>1263.422700929403</v>
       </c>
       <c r="X6">
-        <v>572.2417744532756</v>
+        <v>1714.230368964912</v>
       </c>
       <c r="Y6">
-        <v>1.136202795368727</v>
+        <v>2.729644126140211</v>
       </c>
       <c r="Z6">
-        <v>1410.073778981529</v>
+        <v>1408.908891015012</v>
       </c>
       <c r="AA6">
-        <v>779.2260699897165</v>
+        <v>2179.857334287006</v>
       </c>
       <c r="AB6">
-        <v>0.9510010329105156</v>
+        <v>1.970622915350129</v>
+      </c>
+      <c r="AC6">
+        <v>1369.74693251618</v>
+      </c>
+      <c r="AD6">
+        <v>250.6281626828163</v>
+      </c>
+      <c r="AE6">
+        <v>0.4822530664795167</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -1078,79 +1108,88 @@
         <v>35</v>
       </c>
       <c r="C7">
-        <v>102.8337605786535</v>
+        <v>104.0699802474232</v>
       </c>
       <c r="D7">
-        <v>1286.448209315232</v>
+        <v>1283.528720021782</v>
       </c>
       <c r="E7">
-        <v>2444.703511040217</v>
+        <v>3496.640403516598</v>
       </c>
       <c r="F7">
-        <v>1286.448259317732</v>
+        <v>1283.528770024282</v>
       </c>
       <c r="G7">
-        <v>3858.812974093238</v>
+        <v>11392.63629798917</v>
       </c>
       <c r="H7">
-        <v>0.6592466160249062</v>
+        <v>1.211448030208742</v>
       </c>
       <c r="I7">
-        <v>5.315788071035535</v>
+        <v>6.392279341023214</v>
       </c>
       <c r="J7">
-        <v>0.3440511766497729</v>
+        <v>0.6490916893579486</v>
       </c>
       <c r="K7">
-        <v>1.318493232049812</v>
+        <v>2.422896060417485</v>
       </c>
       <c r="L7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M7">
-        <v>1389.282069898885</v>
+        <v>1387.598300249204</v>
       </c>
       <c r="N7">
-        <v>3849.6732697917</v>
+        <v>7167.795250902307</v>
       </c>
       <c r="O7">
-        <v>1389.282019896385</v>
+        <v>1387.598750271705</v>
       </c>
       <c r="P7">
-        <v>5613.979995898304</v>
+        <v>18793.49647341312</v>
       </c>
       <c r="Q7">
-        <v>0.6108909398936515</v>
+        <v>0.9667401782966623</v>
       </c>
       <c r="S7">
-        <v>5.806857737629341</v>
+        <v>10.47267589855528</v>
       </c>
       <c r="T7">
-        <v>0.3356961831725033</v>
+        <v>0.6721252114051595</v>
       </c>
       <c r="U7">
-        <v>1.221781879787303</v>
+        <v>1.933480356593325</v>
       </c>
       <c r="V7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W7">
-        <v>1266.173669709439</v>
+        <v>1263.492585932036</v>
       </c>
       <c r="X7">
-        <v>410.1414484325996</v>
+        <v>1640.622073592483</v>
       </c>
       <c r="Y7">
-        <v>0.7778213812129449</v>
+        <v>2.789118023363323</v>
       </c>
       <c r="Z7">
-        <v>1410.546291935178</v>
+        <v>1408.947332361973</v>
       </c>
       <c r="AA7">
-        <v>558.2755719733433</v>
+        <v>2180.840684141683</v>
       </c>
       <c r="AB7">
-        <v>0.6705600612440705</v>
+        <v>2.069672803749829</v>
+      </c>
+      <c r="AC7">
+        <v>1369.749857507399</v>
+      </c>
+      <c r="AD7">
+        <v>304.686942076123</v>
+      </c>
+      <c r="AE7">
+        <v>0.4823752353132397</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -1161,79 +1200,88 @@
         <v>36</v>
       </c>
       <c r="C8">
-        <v>103.7653078142782</v>
+        <v>104.0262199914605</v>
       </c>
       <c r="D8">
-        <v>1284.202596464801</v>
+        <v>1283.619840016963</v>
       </c>
       <c r="E8">
-        <v>2088.636569967997</v>
+        <v>3202.18075661169</v>
       </c>
       <c r="F8">
-        <v>1284.202646467301</v>
+        <v>1283.619890019463</v>
       </c>
       <c r="G8">
-        <v>6634.942668099018</v>
+        <v>10417.74882714296</v>
       </c>
       <c r="H8">
-        <v>1.231786936692311</v>
+        <v>1.226506743744636</v>
       </c>
       <c r="I8">
-        <v>4.16063570080835</v>
+        <v>5.547557347563675</v>
       </c>
       <c r="J8">
-        <v>0.5427123771487803</v>
+        <v>0.6147135151406715</v>
       </c>
       <c r="K8">
-        <v>2.463573873384622</v>
+        <v>2.453013487489272</v>
       </c>
       <c r="L8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M8">
-        <v>1387.968004284079</v>
+        <v>1387.646060008424</v>
       </c>
       <c r="N8">
-        <v>4295.932349155232</v>
+        <v>6590.467088729933</v>
       </c>
       <c r="O8">
-        <v>1387.967954281579</v>
+        <v>1387.646110010924</v>
       </c>
       <c r="P8">
-        <v>10925.05487409746</v>
+        <v>17064.57074239271</v>
       </c>
       <c r="Q8">
-        <v>0.9473950998158533</v>
+        <v>0.9696075320511903</v>
       </c>
       <c r="S8">
-        <v>10.31237810448728</v>
+        <v>6.184306606946122</v>
       </c>
       <c r="T8">
-        <v>0.6426458252510582</v>
+        <v>0.6389394328487654</v>
       </c>
       <c r="U8">
-        <v>1.894790199631707</v>
+        <v>1.939215064102381</v>
       </c>
       <c r="V8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W8">
-        <v>1264.184912884582</v>
+        <v>1263.579979470996</v>
       </c>
       <c r="X8">
-        <v>764.110283878153</v>
+        <v>1457.025863862369</v>
       </c>
       <c r="Y8">
-        <v>1.891286460079062</v>
+        <v>2.655689348987981</v>
       </c>
       <c r="Z8">
-        <v>1409.381576306018</v>
+        <v>1409.056322715212</v>
       </c>
       <c r="AA8">
-        <v>1200.20308668871</v>
+        <v>1799.453520624642</v>
       </c>
       <c r="AB8">
-        <v>1.62493585447047</v>
+        <v>1.818998251893742</v>
+      </c>
+      <c r="AC8">
+        <v>1369.81254086962</v>
+      </c>
+      <c r="AD8">
+        <v>206.0747366694999</v>
+      </c>
+      <c r="AE8">
+        <v>0.4834930699488314</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1244,79 +1292,88 @@
         <v>37</v>
       </c>
       <c r="C9">
-        <v>103.4263437983614</v>
+        <v>103.9610700089245</v>
       </c>
       <c r="D9">
-        <v>1284.979609425719</v>
+        <v>1283.770138960355</v>
       </c>
       <c r="E9">
-        <v>2296.667080374208</v>
+        <v>2944.590663542221</v>
       </c>
       <c r="F9">
-        <v>1284.979659428219</v>
+        <v>1283.770188962855</v>
       </c>
       <c r="G9">
-        <v>6261.023675935043</v>
+        <v>9590.581062057307</v>
       </c>
       <c r="H9">
-        <v>1.036070304195946</v>
+        <v>1.235781424175911</v>
       </c>
       <c r="I9">
-        <v>5.716933049101491</v>
+        <v>5.077754320888648</v>
       </c>
       <c r="J9">
-        <v>0.5931105457361748</v>
+        <v>0.5987375986248374</v>
       </c>
       <c r="K9">
-        <v>2.072140608391892</v>
+        <v>2.471562848351821</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M9">
-        <v>1388.40605322908</v>
+        <v>1387.73120896928</v>
       </c>
       <c r="N9">
-        <v>4442.55729364278</v>
+        <v>6072.58799997058</v>
       </c>
       <c r="O9">
-        <v>1388.40600322658</v>
+        <v>1387.73125897178</v>
       </c>
       <c r="P9">
-        <v>9859.409618588685</v>
+        <v>15631.02552956834</v>
       </c>
       <c r="Q9">
-        <v>0.8366850187562342</v>
+        <v>0.9677433139724543</v>
       </c>
       <c r="S9">
-        <v>8.888263058208192</v>
+        <v>5.950834641924713</v>
       </c>
       <c r="T9">
-        <v>0.6128679719406341</v>
+        <v>0.6295543127169215</v>
       </c>
       <c r="U9">
-        <v>1.673370037512468</v>
+        <v>1.935486627944909</v>
       </c>
       <c r="V9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W9">
-        <v>1264.829020225721</v>
+        <v>1263.738007877998</v>
       </c>
       <c r="X9">
-        <v>694.5115592132486</v>
+        <v>1348.378866000947</v>
       </c>
       <c r="Y9">
-        <v>1.501499395216064</v>
+        <v>2.63325350105933</v>
       </c>
       <c r="Z9">
-        <v>1409.784746378137</v>
+        <v>1409.158255295046</v>
       </c>
       <c r="AA9">
-        <v>1059.2723335787</v>
+        <v>1648.221848763337</v>
       </c>
       <c r="AB9">
-        <v>1.239552310763531</v>
+        <v>1.720879161146091</v>
+      </c>
+      <c r="AC9">
+        <v>1369.814374519566</v>
+      </c>
+      <c r="AD9">
+        <v>187.8785610392232</v>
+      </c>
+      <c r="AE9">
+        <v>0.4822769128938145</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1327,79 +1384,88 @@
         <v>38</v>
       </c>
       <c r="C10">
-        <v>103.3933857063571</v>
+        <v>103.8723368591659</v>
       </c>
       <c r="D10">
-        <v>1285.059565981481</v>
+        <v>1283.955805802481</v>
       </c>
       <c r="E10">
-        <v>2315.940513475357</v>
+        <v>2394.985528527229</v>
       </c>
       <c r="F10">
-        <v>1285.059615983981</v>
+        <v>1283.955855804981</v>
       </c>
       <c r="G10">
-        <v>6099.944164391186</v>
+        <v>7833.388160007933</v>
       </c>
       <c r="H10">
-        <v>1.000782908456885</v>
+        <v>1.243795095463287</v>
       </c>
       <c r="I10">
-        <v>5.405742819622261</v>
+        <v>4.565637986913248</v>
       </c>
       <c r="J10">
-        <v>0.5936197501745702</v>
+        <v>0.5930568295363503</v>
       </c>
       <c r="K10">
-        <v>2.00156581691377</v>
+        <v>2.487590190926574</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M10">
-        <v>1388.453051692838</v>
+        <v>1387.828142661647</v>
       </c>
       <c r="N10">
-        <v>4443.65447286676</v>
+        <v>4951.053042229346</v>
       </c>
       <c r="O10">
-        <v>1388.453001690338</v>
+        <v>1387.828192664147</v>
       </c>
       <c r="P10">
-        <v>9568.193787223929</v>
+        <v>12641.02688617835</v>
       </c>
       <c r="Q10">
-        <v>0.8118197849659325</v>
+        <v>0.9625199188294873</v>
       </c>
       <c r="S10">
-        <v>9.31552499609769</v>
+        <v>4.970861207770139</v>
       </c>
       <c r="T10">
-        <v>0.6126850072657607</v>
+        <v>0.6223562237273779</v>
       </c>
       <c r="U10">
-        <v>1.623639569931865</v>
+        <v>1.925039837658975</v>
       </c>
       <c r="V10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W10">
-        <v>1264.975557793525</v>
+        <v>1263.951995419847</v>
       </c>
       <c r="X10">
-        <v>672.6379771613101</v>
+        <v>1100.031747248079</v>
       </c>
       <c r="Y10">
-        <v>1.442794798678854</v>
+        <v>2.591577008201627</v>
       </c>
       <c r="Z10">
-        <v>1409.83970570295</v>
+        <v>1409.223309461557</v>
       </c>
       <c r="AA10">
-        <v>1037.303889605206</v>
+        <v>1317.499846459955</v>
       </c>
       <c r="AB10">
-        <v>1.180139054617655</v>
+        <v>1.619547257406603</v>
+      </c>
+      <c r="AC10">
+        <v>1370.048445547334</v>
+      </c>
+      <c r="AD10">
+        <v>150.266068615093</v>
+      </c>
+      <c r="AE10">
+        <v>0.4796566765674015</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1410,79 +1476,88 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>103.4549277543229</v>
+        <v>103.7654615247409</v>
       </c>
       <c r="D11">
-        <v>1284.906042501789</v>
+        <v>1284.202662424019</v>
       </c>
       <c r="E11">
-        <v>2312.785129461631</v>
+        <v>2096.2345719594</v>
       </c>
       <c r="F11">
-        <v>1284.906092504289</v>
+        <v>1284.202712426519</v>
       </c>
       <c r="G11">
-        <v>6428.82716883244</v>
+        <v>6718.605442260827</v>
       </c>
       <c r="H11">
-        <v>1.069110856278908</v>
+        <v>1.230729184651142</v>
       </c>
       <c r="I11">
-        <v>5.411241116988647</v>
+        <v>4.506459307326285</v>
       </c>
       <c r="J11">
-        <v>0.5630013624533229</v>
+        <v>0.5680576163002561</v>
       </c>
       <c r="K11">
-        <v>2.138221712557816</v>
+        <v>2.461458369302283</v>
       </c>
       <c r="L11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M11">
-        <v>1388.361070261112</v>
+        <v>1387.96812394876</v>
       </c>
       <c r="N11">
-        <v>4564.275872259502</v>
+        <v>4288.96288324252</v>
       </c>
       <c r="O11">
-        <v>1388.361020258611</v>
+        <v>1387.96817395126</v>
       </c>
       <c r="P11">
-        <v>10257.31644767499</v>
+        <v>10735.02426708248</v>
       </c>
       <c r="Q11">
-        <v>0.8470319975568197</v>
+        <v>0.9486025660912757</v>
       </c>
       <c r="S11">
-        <v>10.56757693502368</v>
+        <v>5.099277391885821</v>
       </c>
       <c r="T11">
-        <v>0.6134879218929026</v>
+        <v>0.6079926011571101</v>
       </c>
       <c r="U11">
-        <v>1.694063995113639</v>
+        <v>1.897205132182551</v>
       </c>
       <c r="V11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W11">
-        <v>1264.776888698872</v>
+        <v>1264.163347648316</v>
       </c>
       <c r="X11">
-        <v>704.4241955298553</v>
+        <v>893.8195324510608</v>
       </c>
       <c r="Y11">
-        <v>1.527250943765862</v>
+        <v>2.208594905858877</v>
       </c>
       <c r="Z11">
-        <v>1409.740257228385</v>
+        <v>1409.399833284844</v>
       </c>
       <c r="AA11">
-        <v>1088.883945605306</v>
+        <v>1144.081976203222</v>
       </c>
       <c r="AB11">
-        <v>1.266856239018401</v>
+        <v>1.545895845057688</v>
+      </c>
+      <c r="AC11">
+        <v>1370.135731590343</v>
+      </c>
+      <c r="AD11">
+        <v>144.6536692866076</v>
+      </c>
+      <c r="AE11">
+        <v>0.4729089248574131</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1493,79 +1568,88 @@
         <v>40</v>
       </c>
       <c r="C12">
-        <v>103.5036122422252</v>
+        <v>103.6685841037647</v>
       </c>
       <c r="D12">
-        <v>1284.813737274937</v>
+        <v>1284.419380253633</v>
       </c>
       <c r="E12">
-        <v>2384.501888510541</v>
+        <v>1870.770809230212</v>
       </c>
       <c r="F12">
-        <v>1284.813787277438</v>
+        <v>1284.419430256133</v>
       </c>
       <c r="G12">
-        <v>6825.001413239464</v>
+        <v>5865.884239370888</v>
       </c>
       <c r="H12">
-        <v>1.10552305258791</v>
+        <v>1.205276996529465</v>
       </c>
       <c r="I12">
-        <v>5.978151173904269</v>
+        <v>4.975075524184917</v>
       </c>
       <c r="J12">
-        <v>0.5524050646783379</v>
+        <v>0.5655126981595711</v>
       </c>
       <c r="K12">
-        <v>2.211046105175821</v>
+        <v>2.410553993058929</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M12">
-        <v>1388.317449522163</v>
+        <v>1388.087964357398</v>
       </c>
       <c r="N12">
-        <v>4779.262035633984</v>
+        <v>3825.791202594277</v>
       </c>
       <c r="O12">
-        <v>1388.317399519663</v>
+        <v>1388.088014359898</v>
       </c>
       <c r="P12">
-        <v>10984.70831078779</v>
+        <v>9286.762526548408</v>
       </c>
       <c r="Q12">
-        <v>0.8633165427029357</v>
+        <v>0.9275480332862174</v>
       </c>
       <c r="S12">
-        <v>11.34450188904895</v>
+        <v>4.638311335193286</v>
       </c>
       <c r="T12">
-        <v>0.6220757553855356</v>
+        <v>0.5880813933040889</v>
       </c>
       <c r="U12">
-        <v>1.726633085405871</v>
+        <v>1.855096066572435</v>
       </c>
       <c r="V12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W12">
-        <v>1264.742877754306</v>
+        <v>1264.344628181567</v>
       </c>
       <c r="X12">
-        <v>799.4033515991606</v>
+        <v>836.3203702531307</v>
       </c>
       <c r="Y12">
-        <v>1.62513844784849</v>
+        <v>2.211753344023522</v>
       </c>
       <c r="Z12">
-        <v>1409.683448719498</v>
+        <v>1409.475846529985</v>
       </c>
       <c r="AA12">
-        <v>1173.989231084137</v>
+        <v>996.4364137504804</v>
       </c>
       <c r="AB12">
-        <v>1.30427911768261</v>
+        <v>1.465067369478681</v>
+      </c>
+      <c r="AC12">
+        <v>1370.167009325038</v>
+      </c>
+      <c r="AD12">
+        <v>119.1941050657327</v>
+      </c>
+      <c r="AE12">
+        <v>0.462558448726945</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1576,79 +1660,88 @@
         <v>41</v>
       </c>
       <c r="C13">
-        <v>103.2707279700105</v>
+        <v>103.6034446239503</v>
       </c>
       <c r="D13">
-        <v>1285.368012856323</v>
+        <v>1284.568956535589</v>
       </c>
       <c r="E13">
-        <v>2442.245228843793</v>
+        <v>2592.859374148509</v>
       </c>
       <c r="F13">
-        <v>1285.368062858823</v>
+        <v>1284.569006538089</v>
       </c>
       <c r="G13">
-        <v>5808.778779755517</v>
+        <v>7878.259368471651</v>
       </c>
       <c r="H13">
-        <v>0.909703200198021</v>
+        <v>1.158372393175307</v>
       </c>
       <c r="I13">
-        <v>4.586505782131321</v>
+        <v>6.349439811402313</v>
       </c>
       <c r="J13">
-        <v>0.5768867676552792</v>
+        <v>0.586085265130992</v>
       </c>
       <c r="K13">
-        <v>1.819406400396042</v>
+        <v>2.316744786350615</v>
       </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M13">
-        <v>1388.638840831334</v>
+        <v>1388.171501114537</v>
       </c>
       <c r="N13">
-        <v>4536.42722363767</v>
+        <v>5246.593149543389</v>
       </c>
       <c r="O13">
-        <v>1388.638790828834</v>
+        <v>1388.172451162039</v>
       </c>
       <c r="P13">
-        <v>9014.446755604509</v>
+        <v>12380.59194457184</v>
       </c>
       <c r="Q13">
-        <v>0.7608094256450597</v>
+        <v>0.9031623254334149</v>
       </c>
       <c r="S13">
-        <v>7.44709265947525</v>
+        <v>9.272582083447691</v>
       </c>
       <c r="T13">
-        <v>0.5739710559941704</v>
+        <v>0.5909042382317267</v>
       </c>
       <c r="U13">
-        <v>1.521618851290119</v>
+        <v>1.80632465086683</v>
       </c>
       <c r="V13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W13">
-        <v>1265.25351034193</v>
+        <v>1264.460722423649</v>
       </c>
       <c r="X13">
-        <v>660.3489749966221</v>
+        <v>1072.453262703836</v>
       </c>
       <c r="Y13">
-        <v>1.271481799874146</v>
+        <v>2.104540658253824</v>
       </c>
       <c r="Z13">
-        <v>1409.999822584967</v>
+        <v>1409.554364841877</v>
       </c>
       <c r="AA13">
-        <v>951.816797840345</v>
+        <v>1374.588439476606</v>
       </c>
       <c r="AB13">
-        <v>1.028781891530562</v>
+        <v>1.42273764087852</v>
+      </c>
+      <c r="AC13">
+        <v>1370.175238379656</v>
+      </c>
+      <c r="AD13">
+        <v>210.6737285150027</v>
+      </c>
+      <c r="AE13">
+        <v>0.4518954891207552</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1659,79 +1752,88 @@
         <v>42</v>
       </c>
       <c r="C14">
-        <v>103.8721856694638</v>
+        <v>103.5464355967958</v>
       </c>
       <c r="D14">
-        <v>1283.955754765577</v>
+        <v>1284.689979714949</v>
       </c>
       <c r="E14">
-        <v>2385.120655654849</v>
+        <v>2486.863602303094</v>
       </c>
       <c r="F14">
-        <v>1283.955804768077</v>
+        <v>1284.690029717449</v>
       </c>
       <c r="G14">
-        <v>7725.044753121364</v>
+        <v>7348.222381186395</v>
       </c>
       <c r="H14">
-        <v>1.244857584783979</v>
+        <v>1.122837387753568</v>
       </c>
       <c r="I14">
-        <v>4.012196799246818</v>
+        <v>5.694594463641767</v>
       </c>
       <c r="J14">
-        <v>0.5654636479465963</v>
+        <v>0.593895983239638</v>
       </c>
       <c r="K14">
-        <v>2.489715169567957</v>
+        <v>2.245674775507135</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M14">
-        <v>1387.82804044004</v>
+        <v>1388.236415311745</v>
       </c>
       <c r="N14">
-        <v>4959.108060529968</v>
+        <v>4936.04598967077</v>
       </c>
       <c r="O14">
-        <v>1387.82799043754</v>
+        <v>1388.236465314245</v>
       </c>
       <c r="P14">
-        <v>12880.54044762637</v>
+        <v>11455.32122241365</v>
       </c>
       <c r="Q14">
-        <v>0.9611201649812853</v>
+        <v>0.887193783214792</v>
       </c>
       <c r="S14">
-        <v>10.62451716899781</v>
+        <v>6.754809596796134</v>
       </c>
       <c r="T14">
-        <v>0.6591794396414981</v>
+        <v>0.586421775860053</v>
       </c>
       <c r="U14">
-        <v>1.922240329962571</v>
+        <v>1.774387566429584</v>
       </c>
       <c r="V14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W14">
-        <v>1263.973454148753</v>
+        <v>1264.584645898154</v>
       </c>
       <c r="X14">
-        <v>912.5588444333318</v>
+        <v>914.0007352461676</v>
       </c>
       <c r="Y14">
-        <v>2.152079459439372</v>
+        <v>1.880180974152528</v>
       </c>
       <c r="Z14">
-        <v>1409.199387769317</v>
+        <v>1409.626397114252</v>
       </c>
       <c r="AA14">
-        <v>1404.698582887514</v>
+        <v>1188.335864990215</v>
       </c>
       <c r="AB14">
-        <v>1.730995745539465</v>
+        <v>1.341454720133672</v>
+      </c>
+      <c r="AC14">
+        <v>1370.198099301957</v>
+      </c>
+      <c r="AD14">
+        <v>3006.48263677155</v>
+      </c>
+      <c r="AE14">
+        <v>0.0675144257630096</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -1742,79 +1844,88 @@
         <v>43</v>
       </c>
       <c r="C15">
-        <v>103.5464391814035</v>
+        <v>103.5034610386997</v>
       </c>
       <c r="D15">
-        <v>1284.689861272702</v>
+        <v>1284.813932455793</v>
       </c>
       <c r="E15">
-        <v>2479.542405379102</v>
+        <v>2395.888894864277</v>
       </c>
       <c r="F15">
-        <v>1284.689911275202</v>
+        <v>1284.813982458293</v>
       </c>
       <c r="G15">
-        <v>7274.737585218469</v>
+        <v>6940.846150134952</v>
       </c>
       <c r="H15">
-        <v>1.123855695591821</v>
+        <v>1.104200894278371</v>
       </c>
       <c r="I15">
-        <v>6.120701192967738</v>
+        <v>6.863568406151087</v>
       </c>
       <c r="J15">
-        <v>0.573441543756921</v>
+        <v>0.5864569057127917</v>
       </c>
       <c r="K15">
-        <v>2.247711391183643</v>
+        <v>2.208401788556743</v>
       </c>
       <c r="L15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M15">
-        <v>1388.236400459105</v>
+        <v>1388.317393494492</v>
       </c>
       <c r="N15">
-        <v>4942.728618881605</v>
+        <v>4772.347680995465</v>
       </c>
       <c r="O15">
-        <v>1388.236350456605</v>
+        <v>1388.317443496992</v>
       </c>
       <c r="P15">
-        <v>11647.12778152116</v>
+        <v>10823.66101505125</v>
       </c>
       <c r="Q15">
-        <v>0.8858554898717053</v>
+        <v>0.8647524658209356</v>
       </c>
       <c r="S15">
-        <v>11.37127564280138</v>
+        <v>6.309545393190865</v>
       </c>
       <c r="T15">
-        <v>0.6200026283194158</v>
+        <v>0.5916936458373327</v>
       </c>
       <c r="U15">
-        <v>1.771710979743411</v>
+        <v>1.729504931641871</v>
       </c>
       <c r="V15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W15">
-        <v>1264.596547540883</v>
+        <v>1264.724124962381</v>
       </c>
       <c r="X15">
-        <v>810.9945127146947</v>
+        <v>956.0073476007238</v>
       </c>
       <c r="Y15">
-        <v>1.667927720809621</v>
+        <v>1.949947804488924</v>
       </c>
       <c r="Z15">
-        <v>1409.617116112445</v>
+        <v>1409.69269113064</v>
       </c>
       <c r="AA15">
-        <v>1234.544697825701</v>
+        <v>1124.862864192505</v>
       </c>
       <c r="AB15">
-        <v>1.358982803225403</v>
+        <v>1.248162162139934</v>
+      </c>
+      <c r="AC15">
+        <v>1370.220439156537</v>
+      </c>
+      <c r="AD15">
+        <v>154.5503118421285</v>
+      </c>
+      <c r="AE15">
+        <v>0.4308772515071835</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -1825,82 +1936,91 @@
         <v>44</v>
       </c>
       <c r="C16">
-        <v>103.3653121080913</v>
+        <v>103.4548927166297</v>
       </c>
       <c r="D16">
-        <v>1285.121593961283</v>
+        <v>1284.906152501624</v>
       </c>
       <c r="E16">
-        <v>2574.607946814574</v>
+        <v>2319.612419790947</v>
       </c>
       <c r="F16">
-        <v>1285.121643963783</v>
+        <v>1284.906202504124</v>
       </c>
       <c r="G16">
-        <v>6660.353815083854</v>
+        <v>6495.369965905759</v>
       </c>
       <c r="H16">
-        <v>0.9880350255731249</v>
+        <v>1.068161034886069</v>
       </c>
       <c r="I16">
-        <v>6.311454494191321</v>
+        <v>5.353649620163191</v>
       </c>
       <c r="J16">
-        <v>0.5806098064600411</v>
+        <v>0.5840781625921007</v>
       </c>
       <c r="K16">
-        <v>1.97607005114625</v>
+        <v>2.136322069772138</v>
       </c>
       <c r="L16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M16">
-        <v>1388.487006074374</v>
+        <v>1388.361045218254</v>
       </c>
       <c r="N16">
-        <v>4887.801745020425</v>
+        <v>4556.609031239377</v>
       </c>
       <c r="O16">
-        <v>1388.486956071874</v>
+        <v>1388.361095220754</v>
       </c>
       <c r="P16">
-        <v>10509.03160430982</v>
+        <v>10112.42060285275</v>
       </c>
       <c r="Q16">
-        <v>0.8096952556885484</v>
+        <v>0.8483667268546804</v>
       </c>
       <c r="S16">
-        <v>21.72699949008526</v>
+        <v>5.882511163612157</v>
       </c>
       <c r="T16">
-        <v>0.6151077275940631</v>
+        <v>0.584107187383161</v>
       </c>
       <c r="U16">
-        <v>1.619390511377097</v>
+        <v>1.696733453709361</v>
       </c>
       <c r="V16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W16">
-        <v>1265.01222866341</v>
+        <v>1264.769349911496</v>
       </c>
       <c r="X16">
-        <v>748.0594944092455</v>
+        <v>794.8882117601399</v>
       </c>
       <c r="Y16">
-        <v>1.413407678284065</v>
+        <v>1.720389144398472</v>
       </c>
       <c r="Z16">
-        <v>1399.875010088117</v>
+        <v>1409.747069691199</v>
       </c>
       <c r="AA16">
-        <v>280.9098135638438</v>
+        <v>1032.395016267005</v>
       </c>
       <c r="AB16">
-        <v>0.1706558367940302</v>
+        <v>1.227446983823853</v>
+      </c>
+      <c r="AC16">
+        <v>1370.259263417743</v>
+      </c>
+      <c r="AD16">
+        <v>135.7982931827146</v>
+      </c>
+      <c r="AE16">
+        <v>0.422891250736478</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:31">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1908,82 +2028,91 @@
         <v>45</v>
       </c>
       <c r="C17">
-        <v>103.6002174884327</v>
+        <v>103.4290466704206</v>
       </c>
       <c r="D17">
-        <v>1284.56881363667</v>
+        <v>1284.979704813659</v>
       </c>
       <c r="E17">
-        <v>2582.546378877818</v>
+        <v>2302.46637349499</v>
       </c>
       <c r="F17">
-        <v>1284.56886363917</v>
+        <v>1284.979754816159</v>
       </c>
       <c r="G17">
-        <v>7771.219606114822</v>
+        <v>6314.852054999379</v>
       </c>
       <c r="H17">
-        <v>1.159621420670223</v>
+        <v>1.035168230030314</v>
       </c>
       <c r="I17">
-        <v>6.149280008860501</v>
+        <v>5.391223399301987</v>
       </c>
       <c r="J17">
-        <v>0.5583595193859363</v>
+        <v>0.6105950259041872</v>
       </c>
       <c r="K17">
-        <v>2.319242841340445</v>
+        <v>2.070336460060629</v>
       </c>
       <c r="L17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M17">
-        <v>1388.169131130103</v>
+        <v>1388.408051449077</v>
       </c>
       <c r="N17">
-        <v>5252.81470249228</v>
+        <v>4434.775503311444</v>
       </c>
       <c r="O17">
-        <v>1388.169081127603</v>
+        <v>1388.408801486579</v>
       </c>
       <c r="P17">
-        <v>12689.44816043414</v>
+        <v>9610.941982158711</v>
       </c>
       <c r="Q17">
-        <v>0.9051949872875229</v>
+        <v>0.8350667626896844</v>
       </c>
       <c r="S17">
-        <v>12.43165669638375</v>
+        <v>6.152450262265064</v>
       </c>
       <c r="T17">
-        <v>0.6281463988608311</v>
+        <v>0.5740385915002849</v>
       </c>
       <c r="U17">
-        <v>1.810389974575046</v>
+        <v>1.670133525379369</v>
       </c>
       <c r="V17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W17">
-        <v>1264.483953616763</v>
+        <v>1264.820043926923</v>
       </c>
       <c r="X17">
-        <v>909.3230327855706</v>
+        <v>773.354969456705</v>
       </c>
       <c r="Y17">
-        <v>1.783498755519146</v>
+        <v>1.671376270888219</v>
       </c>
       <c r="Z17">
-        <v>1409.55718312099</v>
+        <v>1409.784037875986</v>
       </c>
       <c r="AA17">
-        <v>1362.563355275139</v>
+        <v>1049.450136577224</v>
       </c>
       <c r="AB17">
-        <v>1.409951639458995</v>
+        <v>1.228571983960089</v>
+      </c>
+      <c r="AC17">
+        <v>1370.258122637218</v>
+      </c>
+      <c r="AD17">
+        <v>152.3309305573573</v>
+      </c>
+      <c r="AE17">
+        <v>0.4177856094097066</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:31">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1991,82 +2120,91 @@
         <v>46</v>
       </c>
       <c r="C18">
-        <v>102.8590116399655</v>
+        <v>103.3958865241545</v>
       </c>
       <c r="D18">
-        <v>1286.380083314847</v>
+        <v>1285.059648226335</v>
       </c>
       <c r="E18">
-        <v>3191.157646048982</v>
+        <v>2326.325775403602</v>
       </c>
       <c r="F18">
-        <v>1286.380133317347</v>
+        <v>1285.059698228835</v>
       </c>
       <c r="G18">
-        <v>5157.645459694972</v>
+        <v>6193.430362036959</v>
       </c>
       <c r="H18">
-        <v>0.6690082433011757</v>
+        <v>0.9991823249342384</v>
       </c>
       <c r="I18">
-        <v>6.590943261013627</v>
+        <v>5.689031324895395</v>
       </c>
       <c r="J18">
-        <v>0.3686806581840831</v>
+        <v>0.6246584810071578</v>
       </c>
       <c r="K18">
-        <v>1.338016486602351</v>
+        <v>1.998364649868477</v>
       </c>
       <c r="L18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M18">
-        <v>1389.239194959812</v>
+        <v>1388.454934720488</v>
       </c>
       <c r="N18">
-        <v>4928.767076166884</v>
+        <v>4438.324645372283</v>
       </c>
       <c r="O18">
-        <v>1389.239144957312</v>
+        <v>1388.45558475299</v>
       </c>
       <c r="P18">
-        <v>7400.296214205338</v>
+        <v>9360.58949851547</v>
       </c>
       <c r="Q18">
-        <v>0.6218134703453144</v>
+        <v>0.8102400621385542</v>
       </c>
       <c r="S18">
-        <v>7.178245410791932</v>
+        <v>6.952723720342765</v>
       </c>
       <c r="T18">
-        <v>0.3671747852126709</v>
+        <v>0.5799126594325105</v>
       </c>
       <c r="U18">
-        <v>1.243626940690629</v>
+        <v>1.620480124277108</v>
       </c>
       <c r="V18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W18">
-        <v>1266.15067896403</v>
+        <v>1264.968493507926</v>
       </c>
       <c r="X18">
-        <v>549.3928795582793</v>
+        <v>782.8698290575718</v>
       </c>
       <c r="Y18">
-        <v>0.7688812313631141</v>
+        <v>1.666416285706839</v>
       </c>
       <c r="Z18">
-        <v>1410.505904329251</v>
+        <v>1409.83857999507</v>
       </c>
       <c r="AA18">
-        <v>754.7566789660661</v>
+        <v>1042.334872159445</v>
       </c>
       <c r="AB18">
-        <v>0.6652944445726565</v>
+        <v>1.18587134302896</v>
+      </c>
+      <c r="AC18">
+        <v>1370.276912340002</v>
+      </c>
+      <c r="AD18">
+        <v>146.6530081223658</v>
+      </c>
+      <c r="AE18">
+        <v>0.4053822332255889</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:31">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -2074,82 +2212,91 @@
         <v>47</v>
       </c>
       <c r="C19">
-        <v>103.9608594786996</v>
+        <v>103.3651984936437</v>
       </c>
       <c r="D19">
-        <v>1283.770126524463</v>
+        <v>1285.121669425518</v>
       </c>
       <c r="E19">
-        <v>2933.049475025531</v>
+        <v>2583.505034522527</v>
       </c>
       <c r="F19">
-        <v>1283.770176526963</v>
+        <v>1285.121719428018</v>
       </c>
       <c r="G19">
-        <v>9464.592656337074</v>
+        <v>6739.124881628475</v>
       </c>
       <c r="H19">
-        <v>1.236749851927017</v>
+        <v>0.9867919097671034</v>
       </c>
       <c r="I19">
-        <v>4.588290749878068</v>
+        <v>6.469075238352064</v>
       </c>
       <c r="J19">
-        <v>0.5726626999756106</v>
+        <v>0.6048508269376416</v>
       </c>
       <c r="K19">
-        <v>2.473499703854033</v>
+        <v>1.973583819534207</v>
       </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M19">
-        <v>1387.731086008162</v>
+        <v>1388.486967924162</v>
       </c>
       <c r="N19">
-        <v>6084.696412512027</v>
+        <v>4874.701213065076</v>
       </c>
       <c r="O19">
-        <v>1387.731036005662</v>
+        <v>1388.486917921662</v>
       </c>
       <c r="P19">
-        <v>15956.6694781484</v>
+        <v>10229.40311518949</v>
       </c>
       <c r="Q19">
-        <v>0.9662957328193174</v>
+        <v>0.8114368492286042</v>
       </c>
       <c r="S19">
-        <v>13.47095494746224</v>
+        <v>8.764881325110698</v>
       </c>
       <c r="T19">
-        <v>0.6695873712761852</v>
+        <v>0.5605209331457908</v>
       </c>
       <c r="U19">
-        <v>1.932591465638635</v>
+        <v>1.622873698457208</v>
       </c>
       <c r="V19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W19">
-        <v>1263.749825965695</v>
+        <v>1265.00512863148</v>
       </c>
       <c r="X19">
-        <v>1121.384284438344</v>
+        <v>850.0676394328289</v>
       </c>
       <c r="Y19">
-        <v>2.197271006396977</v>
+        <v>1.611328696346821</v>
       </c>
       <c r="Z19">
-        <v>1409.128976765973</v>
+        <v>1409.843364515538</v>
       </c>
       <c r="AA19">
-        <v>1767.284903058326</v>
+        <v>876.4376652791639</v>
       </c>
       <c r="AB19">
-        <v>1.850347352527071</v>
+        <v>1.122665081411407</v>
+      </c>
+      <c r="AC19">
+        <v>1370.29729297774</v>
+      </c>
+      <c r="AD19">
+        <v>140.0749212066819</v>
+      </c>
+      <c r="AE19">
+        <v>0.4044238745252486</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:31">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -2157,82 +2304,91 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>102.8853432799197</v>
+        <v>103.2707426676138</v>
       </c>
       <c r="D20">
-        <v>1286.308066639478</v>
+        <v>1285.368019665874</v>
       </c>
       <c r="E20">
-        <v>3724.295415718951</v>
+        <v>2449.394364685501</v>
       </c>
       <c r="F20">
-        <v>1286.308116641978</v>
+        <v>1285.368069668374</v>
       </c>
       <c r="G20">
-        <v>6250.482163161349</v>
+        <v>5868.98768392407</v>
       </c>
       <c r="H20">
-        <v>0.6901187062543344</v>
+        <v>0.9088279252264715</v>
       </c>
       <c r="I20">
-        <v>6.421137201164308</v>
+        <v>5.148655991354907</v>
       </c>
       <c r="J20">
-        <v>0.3867292387536428</v>
+        <v>0.5980503723946201</v>
       </c>
       <c r="K20">
-        <v>1.380237412508669</v>
+        <v>1.817655850452943</v>
       </c>
       <c r="L20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M20">
-        <v>1389.193509924398</v>
+        <v>1388.638762333488</v>
       </c>
       <c r="N20">
-        <v>5894.174097934425</v>
+        <v>4532.220081779826</v>
       </c>
       <c r="O20">
-        <v>1389.193459921898</v>
+        <v>1388.638812335988</v>
       </c>
       <c r="P20">
-        <v>9055.786490266053</v>
+        <v>8941.974173345456</v>
       </c>
       <c r="Q20">
-        <v>0.6348651694467462</v>
+        <v>0.7612675408209484</v>
       </c>
       <c r="S20">
-        <v>7.703915856315487</v>
+        <v>4.555040155660794</v>
       </c>
       <c r="T20">
-        <v>0.3732980343705388</v>
+        <v>0.5573635933422582</v>
       </c>
       <c r="U20">
-        <v>1.269730338893492</v>
+        <v>1.522535081641897</v>
       </c>
       <c r="V20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W20">
-        <v>1266.050784542536</v>
+        <v>1265.246330653272</v>
       </c>
       <c r="X20">
-        <v>667.9164266719873</v>
+        <v>735.4348375475927</v>
       </c>
       <c r="Y20">
-        <v>0.7493588316488314</v>
+        <v>1.419653698719314</v>
       </c>
       <c r="Z20">
-        <v>1410.465465870373</v>
+        <v>1410.001283582144</v>
       </c>
       <c r="AA20">
-        <v>921.1993519281701</v>
+        <v>915.3379937817498</v>
       </c>
       <c r="AB20">
-        <v>0.6796577497082256</v>
+        <v>1.024594193000118</v>
+      </c>
+      <c r="AC20">
+        <v>1370.615572759239</v>
+      </c>
+      <c r="AD20">
+        <v>117.1595436034023</v>
+      </c>
+      <c r="AE20">
+        <v>0.3800750681205607</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:31">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -2240,82 +2396,91 @@
         <v>49</v>
       </c>
       <c r="C21">
-        <v>104.2503528410989</v>
+        <v>103.1904334166263</v>
       </c>
       <c r="D21">
-        <v>1283.13875607447</v>
+        <v>1285.554138372862</v>
       </c>
       <c r="E21">
-        <v>3178.106071278868</v>
+        <v>2261.142335399419</v>
       </c>
       <c r="F21">
-        <v>1283.13880607697</v>
+        <v>1285.554188375362</v>
       </c>
       <c r="G21">
-        <v>10004.63915903484</v>
+        <v>5029.186841277205</v>
       </c>
       <c r="H21">
-        <v>1.167578241944832</v>
+        <v>0.8441349921600951</v>
       </c>
       <c r="I21">
-        <v>7.455141249528499</v>
+        <v>4.077762736632551</v>
       </c>
       <c r="J21">
-        <v>0.6544481922752075</v>
+        <v>0.5963736513331057</v>
       </c>
       <c r="K21">
-        <v>2.335156483889663</v>
+        <v>1.68826998432019</v>
       </c>
       <c r="L21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M21">
-        <v>1387.389208920569</v>
+        <v>1388.744571789488</v>
       </c>
       <c r="N21">
-        <v>6479.288031514964</v>
+        <v>4071.072220157262</v>
       </c>
       <c r="O21">
-        <v>1387.389158918069</v>
+        <v>1388.744621791988</v>
       </c>
       <c r="P21">
-        <v>17436.44037422802</v>
+        <v>7692.044326226887</v>
       </c>
       <c r="Q21">
-        <v>0.9632187058375141</v>
+        <v>0.7350413193175539</v>
       </c>
       <c r="S21">
-        <v>12.64626731736267</v>
+        <v>4.201273118232938</v>
       </c>
       <c r="T21">
-        <v>0.7394186271640977</v>
+        <v>0.5343845069426606</v>
       </c>
       <c r="U21">
-        <v>1.926437411675028</v>
+        <v>1.470082638635108</v>
       </c>
       <c r="V21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W21">
-        <v>1263.131707640568</v>
+        <v>1265.417645231991</v>
       </c>
       <c r="X21">
-        <v>1200.698800663039</v>
+        <v>631.73808221389</v>
       </c>
       <c r="Y21">
-        <v>2.433678938773827</v>
+        <v>1.254128767041955</v>
       </c>
       <c r="Z21">
-        <v>1408.719930777953</v>
+        <v>1410.073373753257</v>
       </c>
       <c r="AA21">
-        <v>1943.390818795554</v>
+        <v>779.313805204835</v>
       </c>
       <c r="AB21">
-        <v>2.189622779119542</v>
+        <v>0.9512848129187762</v>
+      </c>
+      <c r="AC21">
+        <v>1370.671464690019</v>
+      </c>
+      <c r="AD21">
+        <v>116.6256156896269</v>
+      </c>
+      <c r="AE21">
+        <v>0.3669395073969013</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:31">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2323,82 +2488,91 @@
         <v>50</v>
       </c>
       <c r="C22">
-        <v>104.0259342194613</v>
+        <v>103.1253487362933</v>
       </c>
       <c r="D22">
-        <v>1283.619888030458</v>
+        <v>1285.703629441643</v>
       </c>
       <c r="E22">
-        <v>3192.212214066702</v>
+        <v>2057.600170047308</v>
       </c>
       <c r="F22">
-        <v>1283.619938032958</v>
+        <v>1285.703679444143</v>
       </c>
       <c r="G22">
-        <v>10309.98604600376</v>
+        <v>4380.323645124216</v>
       </c>
       <c r="H22">
-        <v>1.227146899557516</v>
+        <v>0.820685858485398</v>
       </c>
       <c r="I22">
-        <v>6.110272419647478</v>
+        <v>3.748518651876895</v>
       </c>
       <c r="J22">
-        <v>0.5945713310730159</v>
+        <v>0.5567851779710523</v>
       </c>
       <c r="K22">
-        <v>2.454293799115033</v>
+        <v>1.641371716970796</v>
       </c>
       <c r="L22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M22">
-        <v>1387.645922254919</v>
+        <v>1388.828978177936</v>
       </c>
       <c r="N22">
-        <v>6602.443982915314</v>
+        <v>3709.054930805649</v>
       </c>
       <c r="O22">
-        <v>1387.645872252419</v>
+        <v>1388.829028180436</v>
       </c>
       <c r="P22">
-        <v>17404.02725375863</v>
+        <v>6742.470242066399</v>
       </c>
       <c r="Q22">
-        <v>0.9685379550258451</v>
+        <v>0.7107095036410981</v>
       </c>
       <c r="S22">
-        <v>14.13409037786169</v>
+        <v>3.58857238591764</v>
       </c>
       <c r="T22">
-        <v>0.6765245541708427</v>
+        <v>0.5215701427342364</v>
       </c>
       <c r="U22">
-        <v>1.93707591005169</v>
+        <v>1.421419007282196</v>
       </c>
       <c r="V22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W22">
-        <v>1263.591775314961</v>
+        <v>1265.547243029865</v>
       </c>
       <c r="X22">
-        <v>1230.904085074818</v>
+        <v>521.4001014808708</v>
       </c>
       <c r="Y22">
-        <v>2.246861204058233</v>
+        <v>1.180471053790343</v>
       </c>
       <c r="Z22">
-        <v>1409.02894749706</v>
+        <v>1410.087435833742</v>
       </c>
       <c r="AA22">
-        <v>1898.190482865157</v>
+        <v>667.1099141427552</v>
       </c>
       <c r="AB22">
-        <v>1.926947122812311</v>
+        <v>0.8700820645524422</v>
+      </c>
+      <c r="AC22">
+        <v>1370.676343356751</v>
+      </c>
+      <c r="AD22">
+        <v>92.00865894182216</v>
+      </c>
+      <c r="AE22">
+        <v>0.3549354301510427</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:31">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -2406,82 +2580,91 @@
         <v>51</v>
       </c>
       <c r="C23">
-        <v>104.0681758352796</v>
+        <v>103.0191573463221</v>
       </c>
       <c r="D23">
-        <v>1283.528701128697</v>
+        <v>1285.956334441275</v>
       </c>
       <c r="E23">
-        <v>3482.103058526789</v>
+        <v>7074.834389602524</v>
       </c>
       <c r="F23">
-        <v>1283.528751131197</v>
+        <v>1285.956384443775</v>
       </c>
       <c r="G23">
-        <v>11235.7517707482</v>
+        <v>13743.67869155332</v>
       </c>
       <c r="H23">
-        <v>1.212290919863234</v>
+        <v>0.7651281165860977</v>
       </c>
       <c r="I23">
-        <v>6.695093930404515</v>
+        <v>10.21865111264668</v>
       </c>
       <c r="J23">
-        <v>0.6226460648296063</v>
+        <v>0.5014342506996523</v>
       </c>
       <c r="K23">
-        <v>2.424581839726469</v>
+        <v>1.530256233172195</v>
       </c>
       <c r="L23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M23">
-        <v>1387.596976968977</v>
+        <v>1388.975491787597</v>
       </c>
       <c r="N23">
-        <v>7170.853383508797</v>
+        <v>12148.83901364465</v>
       </c>
       <c r="O23">
-        <v>1387.596926966477</v>
+        <v>1388.975541790097</v>
       </c>
       <c r="P23">
-        <v>18953.65693286311</v>
+        <v>20609.31749724491</v>
       </c>
       <c r="Q23">
-        <v>0.9663283863696748</v>
+        <v>0.6796018330982188</v>
       </c>
       <c r="S23">
-        <v>15.2959558246701</v>
+        <v>10.39961950448355</v>
       </c>
       <c r="T23">
-        <v>0.6886833402631802</v>
+        <v>0.4585926623520182</v>
       </c>
       <c r="U23">
-        <v>1.93265677273935</v>
+        <v>1.359203666196438</v>
       </c>
       <c r="V23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W23">
-        <v>1263.506560426808</v>
+        <v>1265.750027561093</v>
       </c>
       <c r="X23">
-        <v>1343.032511661094</v>
+        <v>1612.386098352356</v>
       </c>
       <c r="Y23">
-        <v>2.28811152991113</v>
+        <v>0.9732088626329441</v>
       </c>
       <c r="Z23">
-        <v>1408.953602023269</v>
+        <v>1410.265535059281</v>
       </c>
       <c r="AA23">
-        <v>2122.614184771586</v>
+        <v>2134.189936341956</v>
       </c>
       <c r="AB23">
-        <v>2.017162643563402</v>
+        <v>0.8315097774983171</v>
+      </c>
+      <c r="AC23">
+        <v>1370.712591148155</v>
+      </c>
+      <c r="AD23">
+        <v>315.5715278459523</v>
+      </c>
+      <c r="AE23">
+        <v>0.339302348008895</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:31">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -2489,82 +2672,91 @@
         <v>52</v>
       </c>
       <c r="C24">
-        <v>102.9200125636428</v>
+        <v>102.9774673671077</v>
       </c>
       <c r="D24">
-        <v>1286.225763490248</v>
+        <v>1286.056114343005</v>
       </c>
       <c r="E24">
-        <v>4270.03936230286</v>
+        <v>6189.35048261529</v>
       </c>
       <c r="F24">
-        <v>1286.225813492748</v>
+        <v>1286.056164345505</v>
       </c>
       <c r="G24">
-        <v>7319.144269080014</v>
+        <v>11489.09315998306</v>
       </c>
       <c r="H24">
-        <v>0.6906052903683755</v>
+        <v>0.7367637231368613</v>
       </c>
       <c r="I24">
-        <v>7.924953965688293</v>
+        <v>7.443353102800574</v>
       </c>
       <c r="J24">
-        <v>0.441563571510289</v>
+        <v>0.4812922514703085</v>
       </c>
       <c r="K24">
-        <v>1.381210580736751</v>
+        <v>1.473527446273723</v>
       </c>
       <c r="L24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M24">
-        <v>1389.145876058891</v>
+        <v>1389.033781720113</v>
       </c>
       <c r="N24">
-        <v>6777.347169414379</v>
+        <v>10276.20555574801</v>
       </c>
       <c r="O24">
-        <v>1389.145826056391</v>
+        <v>1389.033631712613</v>
       </c>
       <c r="P24">
-        <v>10690.55379313373</v>
+        <v>16882.280002819</v>
       </c>
       <c r="Q24">
-        <v>0.6506779353119985</v>
+        <v>0.6707130773314649</v>
       </c>
       <c r="S24">
-        <v>8.816204241639426</v>
+        <v>9.379834826200804</v>
       </c>
       <c r="T24">
-        <v>0.3780468675968379</v>
+        <v>0.4173198410762562</v>
       </c>
       <c r="U24">
-        <v>1.301355870623997</v>
+        <v>1.34142615466293</v>
       </c>
       <c r="V24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W24">
-        <v>1266.013441612187</v>
+        <v>1265.843088675812</v>
       </c>
       <c r="X24">
-        <v>783.5196943746174</v>
+        <v>1309.914547309592</v>
       </c>
       <c r="Y24">
-        <v>0.8159180363181043</v>
+        <v>0.9156051883878639</v>
       </c>
       <c r="Z24">
-        <v>1410.420013763752</v>
+        <v>1410.325321894831</v>
       </c>
       <c r="AA24">
-        <v>1106.856130917077</v>
+        <v>1765.398155827131</v>
       </c>
       <c r="AB24">
-        <v>0.7474183120179975</v>
+        <v>0.7939612365707055</v>
+      </c>
+      <c r="AC24">
+        <v>1370.735471287282</v>
+      </c>
+      <c r="AD24">
+        <v>282.7257809772601</v>
+      </c>
+      <c r="AE24">
+        <v>0.3358374974747175</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:31">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -2572,82 +2764,91 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>104.3058546353907</v>
+        <v>102.95120616855</v>
       </c>
       <c r="D25">
-        <v>1283.014026088606</v>
+        <v>1286.13693517134</v>
       </c>
       <c r="E25">
-        <v>3836.873252098485</v>
+        <v>4876.942186401248</v>
       </c>
       <c r="F25">
-        <v>1283.014076091106</v>
+        <v>1286.13698517384</v>
       </c>
       <c r="G25">
-        <v>11938.10731553963</v>
+        <v>8732.096736990719</v>
       </c>
       <c r="H25">
-        <v>1.13435481400706</v>
+        <v>0.7122490503097596</v>
       </c>
       <c r="I25">
-        <v>8.408727678445336</v>
+        <v>7.517944556504363</v>
       </c>
       <c r="J25">
-        <v>0.6962034109650834</v>
+        <v>0.4753784336954161</v>
       </c>
       <c r="K25">
-        <v>2.268709628014119</v>
+        <v>1.424498100619519</v>
       </c>
       <c r="L25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M25">
-        <v>1387.319980728997</v>
+        <v>1389.088341349891</v>
       </c>
       <c r="N25">
-        <v>7651.696076814492</v>
+        <v>7891.755255656003</v>
       </c>
       <c r="O25">
-        <v>1387.319930726497</v>
+        <v>1389.08819134239</v>
       </c>
       <c r="P25">
-        <v>20721.18136275716</v>
+        <v>12482.00189285986</v>
       </c>
       <c r="Q25">
-        <v>0.9739092166538923</v>
+        <v>0.6553740525191503</v>
       </c>
       <c r="S25">
-        <v>15.56820824875582</v>
+        <v>7.156810177662953</v>
       </c>
       <c r="T25">
-        <v>0.7282336329616301</v>
+        <v>0.3806285614683812</v>
       </c>
       <c r="U25">
-        <v>1.947818433307785</v>
+        <v>1.310748105038301</v>
       </c>
       <c r="V25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W25">
-        <v>1262.983291477722</v>
+        <v>1265.913103808821</v>
       </c>
       <c r="X25">
-        <v>1453.232903650108</v>
+        <v>988.3284366187166</v>
       </c>
       <c r="Y25">
-        <v>2.512883942156782</v>
+        <v>0.8967989129368017</v>
       </c>
       <c r="Z25">
-        <v>1408.63087255069</v>
+        <v>1410.376092945617</v>
       </c>
       <c r="AA25">
-        <v>2356.453837105989</v>
+        <v>1316.32469143559</v>
       </c>
       <c r="AB25">
-        <v>2.307932483247352</v>
+        <v>0.7787164152297118</v>
+      </c>
+      <c r="AC25">
+        <v>1370.727491096516</v>
+      </c>
+      <c r="AD25">
+        <v>198.3123745775959</v>
+      </c>
+      <c r="AE25">
+        <v>0.3284677274690029</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:31">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -2655,82 +2856,91 @@
         <v>54</v>
       </c>
       <c r="C26">
-        <v>104.383362660632</v>
+        <v>102.9189177911881</v>
       </c>
       <c r="D26">
-        <v>1282.850781937653</v>
+        <v>1286.22569615915</v>
       </c>
       <c r="E26">
-        <v>3946.606572081136</v>
+        <v>4274.038069098433</v>
       </c>
       <c r="F26">
-        <v>1282.850831940153</v>
+        <v>1286.22574616165</v>
       </c>
       <c r="G26">
-        <v>12106.21348018715</v>
+        <v>7341.831228728954</v>
       </c>
       <c r="H26">
-        <v>1.107439697260952</v>
+        <v>0.6902178178140592</v>
       </c>
       <c r="I26">
-        <v>9.547476968431155</v>
+        <v>6.786449888934414</v>
       </c>
       <c r="J26">
-        <v>0.7197151651554008</v>
+        <v>0.4488234115761898</v>
       </c>
       <c r="K26">
-        <v>2.214879394521904</v>
+        <v>1.380435635628118</v>
       </c>
       <c r="L26" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M26">
-        <v>1387.234244603285</v>
+        <v>1389.14501397034</v>
       </c>
       <c r="N26">
-        <v>7764.197101736237</v>
+        <v>6771.652095810011</v>
       </c>
       <c r="O26">
-        <v>1387.234194600785</v>
+        <v>1389.144663952839</v>
       </c>
       <c r="P26">
-        <v>21300.73570579229</v>
+        <v>10344.80654084406</v>
       </c>
       <c r="Q26">
-        <v>0.978862273326762</v>
+        <v>0.6474534514397902</v>
       </c>
       <c r="S26">
-        <v>15.9466025658933</v>
+        <v>6.302061264341831</v>
       </c>
       <c r="T26">
-        <v>0.7470235277861224</v>
+        <v>0.3293564980410818</v>
       </c>
       <c r="U26">
-        <v>1.957724546653524</v>
+        <v>1.29490690287958</v>
       </c>
       <c r="V26" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W26">
-        <v>1262.822268452307</v>
+        <v>1266.012272813883</v>
       </c>
       <c r="X26">
-        <v>1495.324801943479</v>
+        <v>816.2798702005875</v>
       </c>
       <c r="Y26">
-        <v>2.58648343098436</v>
+        <v>0.8170425635451808</v>
       </c>
       <c r="Z26">
-        <v>1408.523220078708</v>
+        <v>1410.419960010058</v>
       </c>
       <c r="AA26">
-        <v>2408.279542262295</v>
+        <v>1116.665684604461</v>
       </c>
       <c r="AB26">
-        <v>2.426522148693881</v>
+        <v>0.7473874027881375</v>
+      </c>
+      <c r="AC26">
+        <v>1370.771140052243</v>
+      </c>
+      <c r="AD26">
+        <v>167.6996502367559</v>
+      </c>
+      <c r="AE26">
+        <v>0.3251526940531522</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:31">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -2738,494 +2948,88 @@
         <v>55</v>
       </c>
       <c r="C27">
-        <v>104.1081746505163</v>
+        <v>104.3848506183388</v>
       </c>
       <c r="D27">
-        <v>1283.442706033513</v>
+        <v>1282.850769784342</v>
       </c>
       <c r="E27">
-        <v>3714.030458324617</v>
+        <v>3956.226356901389</v>
       </c>
       <c r="F27">
-        <v>1283.442756036013</v>
+        <v>1282.850819786842</v>
       </c>
       <c r="G27">
-        <v>11983.12993862622</v>
+        <v>12198.62525312221</v>
       </c>
       <c r="H27">
-        <v>1.21106089941968</v>
+        <v>1.107141432898475</v>
       </c>
       <c r="I27">
-        <v>7.546450163684939</v>
+        <v>7.262998937532849</v>
       </c>
       <c r="J27">
-        <v>0.624914545782677</v>
+        <v>0.7333322538663276</v>
       </c>
       <c r="K27">
-        <v>2.42212179883936</v>
+        <v>2.21428286579695</v>
       </c>
       <c r="L27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M27">
-        <v>1387.55098068903</v>
+        <v>1387.23542039268</v>
       </c>
       <c r="N27">
-        <v>7710.021458294597</v>
+        <v>7760.766771736794</v>
       </c>
       <c r="O27">
-        <v>1387.550930686529</v>
+        <v>1387.23567040518</v>
       </c>
       <c r="P27">
-        <v>20505.346701116</v>
+        <v>21153.04422503191</v>
       </c>
       <c r="Q27">
-        <v>0.9660593914339188</v>
+        <v>0.9792070274384335</v>
       </c>
       <c r="S27">
-        <v>15.70936540840369</v>
+        <v>10.24833567459562</v>
       </c>
       <c r="T27">
-        <v>0.7043039520139347</v>
+        <v>0.7340112502607719</v>
       </c>
       <c r="U27">
-        <v>1.932118782867838</v>
+        <v>1.958414054876867</v>
       </c>
       <c r="V27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W27">
-        <v>1263.440191558002</v>
+        <v>1262.82220276773</v>
       </c>
       <c r="X27">
-        <v>1413.761922914928</v>
+        <v>1768.290496269398</v>
       </c>
       <c r="Y27">
-        <v>2.253993030751442</v>
+        <v>3.04912787606042</v>
       </c>
       <c r="Z27">
-        <v>1408.874548996317</v>
+        <v>1408.516684815578</v>
       </c>
       <c r="AA27">
-        <v>2314.382524090918</v>
+        <v>2475.13844014026</v>
       </c>
       <c r="AB27">
-        <v>2.089791493238601</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28">
-      <c r="A28" s="1">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28">
-        <v>104.1338603981023</v>
-      </c>
-      <c r="D28">
-        <v>1283.384557098306</v>
-      </c>
-      <c r="E28">
-        <v>4005.599911622949</v>
-      </c>
-      <c r="F28">
-        <v>1283.384607100806</v>
-      </c>
-      <c r="G28">
-        <v>12795.11516074324</v>
-      </c>
-      <c r="H28">
-        <v>1.197063775956233</v>
-      </c>
-      <c r="I28">
-        <v>7.759791203032604</v>
-      </c>
-      <c r="J28">
-        <v>0.6289688800341711</v>
-      </c>
-      <c r="K28">
-        <v>2.394127551912466</v>
-      </c>
-      <c r="L28" t="s">
-        <v>61</v>
-      </c>
-      <c r="M28">
-        <v>1387.518517501409</v>
-      </c>
-      <c r="N28">
-        <v>8276.707790124801</v>
-      </c>
-      <c r="O28">
-        <v>1387.518467498909</v>
-      </c>
-      <c r="P28">
-        <v>22110.19736112231</v>
-      </c>
-      <c r="Q28">
-        <v>0.9691699312500497</v>
-      </c>
-      <c r="S28">
-        <v>16.72212089072437</v>
-      </c>
-      <c r="T28">
-        <v>0.7072002684327299</v>
-      </c>
-      <c r="U28">
-        <v>1.938339862500099</v>
-      </c>
-      <c r="V28" t="s">
-        <v>61</v>
-      </c>
-      <c r="W28">
-        <v>1263.425229158311</v>
-      </c>
-      <c r="X28">
-        <v>1531.665686235839</v>
-      </c>
-      <c r="Y28">
-        <v>2.318311491929252</v>
-      </c>
-      <c r="Z28">
-        <v>1408.8422687121</v>
-      </c>
-      <c r="AA28">
-        <v>2463.025769131883</v>
-      </c>
-      <c r="AB28">
-        <v>2.07990263366272</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28">
-      <c r="A29" s="1">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29">
-        <v>102.9517183629034</v>
-      </c>
-      <c r="D29">
-        <v>1286.13694961249</v>
-      </c>
-      <c r="E29">
-        <v>4872.596735894732</v>
-      </c>
-      <c r="F29">
-        <v>1286.13699961499</v>
-      </c>
-      <c r="G29">
-        <v>8706.815937329673</v>
-      </c>
-      <c r="H29">
-        <v>0.7126319755879689</v>
-      </c>
-      <c r="I29">
-        <v>7.961006502867277</v>
-      </c>
-      <c r="J29">
-        <v>0.4686418496566259</v>
-      </c>
-      <c r="K29">
-        <v>1.425263951175938</v>
-      </c>
-      <c r="L29" t="s">
-        <v>61</v>
-      </c>
-      <c r="M29">
-        <v>1389.088767980393</v>
-      </c>
-      <c r="N29">
-        <v>7895.006019196755</v>
-      </c>
-      <c r="O29">
-        <v>1389.088717977893</v>
-      </c>
-      <c r="P29">
-        <v>12716.53853069459</v>
-      </c>
-      <c r="Q29">
-        <v>0.6573225868309356</v>
-      </c>
-      <c r="S29">
-        <v>9.953887480361974</v>
-      </c>
-      <c r="T29">
-        <v>0.4071494548446039</v>
-      </c>
-      <c r="U29">
-        <v>1.314645173661871</v>
-      </c>
-      <c r="V29" t="s">
-        <v>61</v>
-      </c>
-      <c r="W29">
-        <v>1265.913597567748</v>
-      </c>
-      <c r="X29">
-        <v>943.6044703342452</v>
-      </c>
-      <c r="Y29">
-        <v>0.890879286007246</v>
-      </c>
-      <c r="Z29">
-        <v>1410.37625740096</v>
-      </c>
-      <c r="AA29">
-        <v>1316.491297057702</v>
-      </c>
-      <c r="AB29">
-        <v>0.7786233365899795</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28">
-      <c r="A30" s="1">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30">
-        <v>104.163485090502</v>
-      </c>
-      <c r="D30">
-        <v>1283.321171721677</v>
-      </c>
-      <c r="E30">
-        <v>4278.310882558222</v>
-      </c>
-      <c r="F30">
-        <v>1283.321221724177</v>
-      </c>
-      <c r="G30">
-        <v>13567.58340329488</v>
-      </c>
-      <c r="H30">
-        <v>1.187975458195527</v>
-      </c>
-      <c r="I30">
-        <v>10.51223561481052</v>
-      </c>
-      <c r="J30">
-        <v>0.6299868779173852</v>
-      </c>
-      <c r="K30">
-        <v>2.375950916391053</v>
-      </c>
-      <c r="L30" t="s">
-        <v>61</v>
-      </c>
-      <c r="M30">
-        <v>1387.484756817179</v>
-      </c>
-      <c r="N30">
-        <v>8751.023759629679</v>
-      </c>
-      <c r="O30">
-        <v>1387.484706814679</v>
-      </c>
-      <c r="P30">
-        <v>23363.77018115281</v>
-      </c>
-      <c r="Q30">
-        <v>0.9669075973944692</v>
-      </c>
-      <c r="S30">
-        <v>17.60837636961513</v>
-      </c>
-      <c r="T30">
-        <v>0.7114278160748851</v>
-      </c>
-      <c r="U30">
-        <v>1.933815194788938</v>
-      </c>
-      <c r="V30" t="s">
-        <v>61</v>
-      </c>
-      <c r="W30">
-        <v>1263.28529461889</v>
-      </c>
-      <c r="X30">
-        <v>1645.598782291687</v>
-      </c>
-      <c r="Y30">
-        <v>2.443784647278374</v>
-      </c>
-      <c r="Z30">
-        <v>1408.822946018333</v>
-      </c>
-      <c r="AA30">
-        <v>2603.179579782605</v>
-      </c>
-      <c r="AB30">
-        <v>2.120142779318172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28">
-      <c r="A31" s="1">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31">
-        <v>102.9778393403744</v>
-      </c>
-      <c r="D31">
-        <v>1286.05606139817</v>
-      </c>
-      <c r="E31">
-        <v>6178.639235357078</v>
-      </c>
-      <c r="F31">
-        <v>1286.05611140067</v>
-      </c>
-      <c r="G31">
-        <v>11418.4163749777</v>
-      </c>
-      <c r="H31">
-        <v>0.737327044878932</v>
-      </c>
-      <c r="I31">
-        <v>7.646915379061438</v>
-      </c>
-      <c r="J31">
-        <v>0.4675471180760495</v>
-      </c>
-      <c r="K31">
-        <v>1.474654089757864</v>
-      </c>
-      <c r="L31" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31">
-        <v>1389.034000743544</v>
-      </c>
-      <c r="N31">
-        <v>10280.22947167475</v>
-      </c>
-      <c r="O31">
-        <v>1389.033950741044</v>
-      </c>
-      <c r="P31">
-        <v>17123.08455147898</v>
-      </c>
-      <c r="Q31">
-        <v>0.6721513068535441</v>
-      </c>
-      <c r="S31">
-        <v>13.57102654227374</v>
-      </c>
-      <c r="T31">
-        <v>0.4372638857081367</v>
-      </c>
-      <c r="U31">
-        <v>1.344302613707088</v>
-      </c>
-      <c r="V31" t="s">
-        <v>61</v>
-      </c>
-      <c r="W31">
-        <v>1265.845010067814</v>
-      </c>
-      <c r="X31">
-        <v>1212.095525940197</v>
-      </c>
-      <c r="Y31">
-        <v>0.9074457283528383</v>
-      </c>
-      <c r="Z31">
-        <v>1410.325483265627</v>
-      </c>
-      <c r="AA31">
-        <v>1769.716727294939</v>
-      </c>
-      <c r="AB31">
-        <v>0.7938686688631729</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28">
-      <c r="A32" s="1">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32">
-        <v>103.0190730349002</v>
-      </c>
-      <c r="D32">
-        <v>1285.956316624367</v>
-      </c>
-      <c r="E32">
-        <v>7063.064166233817</v>
-      </c>
-      <c r="F32">
-        <v>1285.956366626867</v>
-      </c>
-      <c r="G32">
-        <v>13656.2982816283</v>
-      </c>
-      <c r="H32">
-        <v>0.7654984391198341</v>
-      </c>
-      <c r="I32">
-        <v>9.123175373935188</v>
-      </c>
-      <c r="J32">
-        <v>0.4878157508932678</v>
-      </c>
-      <c r="K32">
-        <v>1.530996878239668</v>
-      </c>
-      <c r="L32" t="s">
-        <v>61</v>
-      </c>
-      <c r="M32">
-        <v>1388.975489664268</v>
-      </c>
-      <c r="N32">
-        <v>12152.75856546629</v>
-      </c>
-      <c r="O32">
-        <v>1388.975439661767</v>
-      </c>
-      <c r="P32">
-        <v>20690.22504989627</v>
-      </c>
-      <c r="Q32">
-        <v>0.6792699145742058</v>
-      </c>
-      <c r="S32">
-        <v>16.39214920703225</v>
-      </c>
-      <c r="T32">
-        <v>0.4674137492519471</v>
-      </c>
-      <c r="U32">
-        <v>1.358539829148412</v>
-      </c>
-      <c r="V32" t="s">
-        <v>61</v>
-      </c>
-      <c r="W32">
-        <v>1265.752019875825</v>
-      </c>
-      <c r="X32">
-        <v>1501.371369892787</v>
-      </c>
-      <c r="Y32">
-        <v>0.934076586849935</v>
-      </c>
-      <c r="Z32">
-        <v>1410.265362370239</v>
-      </c>
-      <c r="AA32">
-        <v>2161.396915526146</v>
-      </c>
-      <c r="AB32">
-        <v>0.8310961865783317</v>
+        <v>2.487623233437122</v>
+      </c>
+      <c r="AC27">
+        <v>1369.651845742202</v>
+      </c>
+      <c r="AD27">
+        <v>335.1710752135344</v>
+      </c>
+      <c r="AE27">
+        <v>0.488598465863808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>